<commit_message>
Evaluation preparation and scripting
</commit_message>
<xml_diff>
--- a/COBREX-CLI/finaleval.xlsx
+++ b/COBREX-CLI/finaleval.xlsx
@@ -13,14 +13,14 @@
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="88">
   <si>
     <t xml:space="preserve">Sr.No.</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t xml:space="preserve">Noise</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># of total extracted rules</t>
   </si>
   <si>
     <t xml:space="preserve"># of rules when 1 and 2 no t given</t>
@@ -93,6 +96,15 @@
 NUM_DAYS</t>
   </si>
   <si>
+    <t xml:space="preserve">{'ruled', 'evaluate'}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{'close', 'compute', 'move', 'read', 'display', 'perform', 'start', 'open', 'if', 'write', 'stop', 'paragraphName'}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{}</t>
+  </si>
+  <si>
     <t xml:space="preserve">LOANPYMT.cbl</t>
   </si>
   <si>
@@ -105,6 +117,12 @@
     <t xml:space="preserve">monthly-interest
 loan-term-months
 Present-value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">set()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{'move', 'multiply', 'divide', 'display', 'start', 'goto', 'if', 'compute', 'paragraphName', 'accept', 'stop'}</t>
   </si>
   <si>
     <t xml:space="preserve">POKER.cbl</t>
@@ -484,31 +502,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -529,27 +547,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BO129"/>
+  <dimension ref="A1:BP129"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1048573" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1048576" activeCellId="0" sqref="F1048576"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="15.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="17.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="18.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="14" style="0" width="14.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="11.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="16.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="14.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="1" width="17.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="14.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="18.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="15" style="1" width="14.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="11.68"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="90.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -601,7 +619,7 @@
       <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
       <c r="S1" s="3" t="s">
@@ -610,7 +628,9 @@
       <c r="T1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="3"/>
+      <c r="U1" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="V1" s="3"/>
       <c r="W1" s="3"/>
       <c r="X1" s="3"/>
@@ -624,33 +644,50 @@
       <c r="AF1" s="3"/>
       <c r="AG1" s="3"/>
       <c r="AH1" s="3"/>
-    </row>
-    <row r="2" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AI1" s="3"/>
+    </row>
+    <row r="2" customFormat="false" ht="54.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="4"/>
+        <v>21</v>
+      </c>
+      <c r="C2" s="4" t="n">
+        <v>8</v>
+      </c>
       <c r="D2" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+      <c r="H2" s="4" t="n">
+        <v>1</v>
+      </c>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
+      <c r="K2" s="4" t="n">
+        <v>1</v>
+      </c>
       <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
+      <c r="M2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="O2" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="P2" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="R2" s="4"/>
       <c r="S2" s="4"/>
       <c r="T2" s="4"/>
@@ -697,37 +734,54 @@
       <c r="BI2" s="4"/>
       <c r="BJ2" s="4"/>
       <c r="BK2" s="4"/>
-      <c r="BL2" s="6"/>
+      <c r="BL2" s="4"/>
       <c r="BM2" s="6"/>
       <c r="BN2" s="6"/>
       <c r="BO2" s="6"/>
-    </row>
-    <row r="3" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP2" s="6"/>
+    </row>
+    <row r="3" customFormat="false" ht="108.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="4"/>
+        <v>27</v>
+      </c>
+      <c r="C3" s="4" t="n">
+        <v>13</v>
+      </c>
       <c r="D3" s="5" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
+      <c r="H3" s="4" t="n">
+        <v>12</v>
+      </c>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
+      <c r="K3" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
+      <c r="M3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="O3" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="P3" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="R3" s="4"/>
       <c r="S3" s="4"/>
       <c r="T3" s="4"/>
@@ -774,24 +828,25 @@
       <c r="BI3" s="4"/>
       <c r="BJ3" s="4"/>
       <c r="BK3" s="4"/>
-      <c r="BL3" s="6"/>
+      <c r="BL3" s="4"/>
       <c r="BM3" s="6"/>
       <c r="BN3" s="6"/>
       <c r="BO3" s="6"/>
-    </row>
-    <row r="4" customFormat="false" ht="198.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP3" s="6"/>
+    </row>
+    <row r="4" customFormat="false" ht="198" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="5" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
@@ -851,24 +906,25 @@
       <c r="BI4" s="4"/>
       <c r="BJ4" s="4"/>
       <c r="BK4" s="4"/>
-      <c r="BL4" s="6"/>
+      <c r="BL4" s="4"/>
       <c r="BM4" s="6"/>
       <c r="BN4" s="6"/>
       <c r="BO4" s="6"/>
-    </row>
-    <row r="5" customFormat="false" ht="198.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP4" s="6"/>
+    </row>
+    <row r="5" customFormat="false" ht="198" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="5" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
@@ -928,24 +984,25 @@
       <c r="BI5" s="4"/>
       <c r="BJ5" s="4"/>
       <c r="BK5" s="4"/>
-      <c r="BL5" s="6"/>
+      <c r="BL5" s="4"/>
       <c r="BM5" s="6"/>
       <c r="BN5" s="6"/>
       <c r="BO5" s="6"/>
-    </row>
-    <row r="6" customFormat="false" ht="73.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP5" s="6"/>
+    </row>
+    <row r="6" customFormat="false" ht="72.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="5" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
@@ -1005,24 +1062,25 @@
       <c r="BI6" s="4"/>
       <c r="BJ6" s="4"/>
       <c r="BK6" s="4"/>
-      <c r="BL6" s="6"/>
+      <c r="BL6" s="4"/>
       <c r="BM6" s="6"/>
       <c r="BN6" s="6"/>
       <c r="BO6" s="6"/>
-    </row>
-    <row r="7" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP6" s="6"/>
+    </row>
+    <row r="7" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="5" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
@@ -1082,24 +1140,25 @@
       <c r="BI7" s="4"/>
       <c r="BJ7" s="4"/>
       <c r="BK7" s="4"/>
-      <c r="BL7" s="6"/>
+      <c r="BL7" s="4"/>
       <c r="BM7" s="6"/>
       <c r="BN7" s="6"/>
       <c r="BO7" s="6"/>
-    </row>
-    <row r="8" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP7" s="6"/>
+    </row>
+    <row r="8" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="n">
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="5" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
@@ -1159,24 +1218,25 @@
       <c r="BI8" s="4"/>
       <c r="BJ8" s="4"/>
       <c r="BK8" s="4"/>
-      <c r="BL8" s="6"/>
+      <c r="BL8" s="4"/>
       <c r="BM8" s="6"/>
       <c r="BN8" s="6"/>
       <c r="BO8" s="6"/>
-    </row>
-    <row r="9" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP8" s="6"/>
+    </row>
+    <row r="9" customFormat="false" ht="54.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="n">
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="5" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
@@ -1236,24 +1296,25 @@
       <c r="BI9" s="4"/>
       <c r="BJ9" s="4"/>
       <c r="BK9" s="4"/>
-      <c r="BL9" s="6"/>
+      <c r="BL9" s="4"/>
       <c r="BM9" s="6"/>
       <c r="BN9" s="6"/>
       <c r="BO9" s="6"/>
-    </row>
-    <row r="10" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP9" s="6"/>
+    </row>
+    <row r="10" customFormat="false" ht="90.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="n">
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="5" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
@@ -1313,24 +1374,25 @@
       <c r="BI10" s="4"/>
       <c r="BJ10" s="4"/>
       <c r="BK10" s="4"/>
-      <c r="BL10" s="6"/>
+      <c r="BL10" s="4"/>
       <c r="BM10" s="6"/>
       <c r="BN10" s="6"/>
       <c r="BO10" s="6"/>
-    </row>
-    <row r="11" customFormat="false" ht="19.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="BP10" s="6"/>
+    </row>
+    <row r="11" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="n">
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="5" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
@@ -1390,21 +1452,22 @@
       <c r="BI11" s="4"/>
       <c r="BJ11" s="4"/>
       <c r="BK11" s="4"/>
-      <c r="BL11" s="6"/>
+      <c r="BL11" s="4"/>
       <c r="BM11" s="6"/>
       <c r="BN11" s="6"/>
       <c r="BO11" s="6"/>
-    </row>
-    <row r="12" customFormat="false" ht="288.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP11" s="6"/>
+    </row>
+    <row r="12" customFormat="false" ht="288" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="n">
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="5" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="4"/>
@@ -1465,21 +1528,22 @@
       <c r="BI12" s="4"/>
       <c r="BJ12" s="4"/>
       <c r="BK12" s="4"/>
-      <c r="BL12" s="6"/>
+      <c r="BL12" s="4"/>
       <c r="BM12" s="6"/>
       <c r="BN12" s="6"/>
       <c r="BO12" s="6"/>
-    </row>
-    <row r="13" customFormat="false" ht="73.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP12" s="6"/>
+    </row>
+    <row r="13" customFormat="false" ht="72.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="n">
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="5" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="4"/>
@@ -1540,24 +1604,25 @@
       <c r="BI13" s="4"/>
       <c r="BJ13" s="4"/>
       <c r="BK13" s="4"/>
-      <c r="BL13" s="6"/>
+      <c r="BL13" s="4"/>
       <c r="BM13" s="6"/>
       <c r="BN13" s="6"/>
       <c r="BO13" s="6"/>
-    </row>
-    <row r="14" customFormat="false" ht="646.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP13" s="6"/>
+    </row>
+    <row r="14" customFormat="false" ht="645.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="n">
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="5" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
@@ -1617,24 +1682,25 @@
       <c r="BI14" s="4"/>
       <c r="BJ14" s="4"/>
       <c r="BK14" s="4"/>
-      <c r="BL14" s="6"/>
+      <c r="BL14" s="4"/>
       <c r="BM14" s="6"/>
       <c r="BN14" s="6"/>
       <c r="BO14" s="6"/>
-    </row>
-    <row r="15" customFormat="false" ht="431.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP14" s="6"/>
+    </row>
+    <row r="15" customFormat="false" ht="431.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="n">
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="5" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
@@ -1694,24 +1760,25 @@
       <c r="BI15" s="4"/>
       <c r="BJ15" s="4"/>
       <c r="BK15" s="4"/>
-      <c r="BL15" s="6"/>
+      <c r="BL15" s="4"/>
       <c r="BM15" s="6"/>
       <c r="BN15" s="6"/>
       <c r="BO15" s="6"/>
-    </row>
-    <row r="16" customFormat="false" ht="431.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP15" s="6"/>
+    </row>
+    <row r="16" customFormat="false" ht="431.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="n">
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="5" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
@@ -1771,24 +1838,25 @@
       <c r="BI16" s="4"/>
       <c r="BJ16" s="4"/>
       <c r="BK16" s="4"/>
-      <c r="BL16" s="6"/>
+      <c r="BL16" s="4"/>
       <c r="BM16" s="6"/>
       <c r="BN16" s="6"/>
       <c r="BO16" s="6"/>
-    </row>
-    <row r="17" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP16" s="6"/>
+    </row>
+    <row r="17" customFormat="false" ht="90.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="n">
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="5" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
@@ -1848,24 +1916,25 @@
       <c r="BI17" s="4"/>
       <c r="BJ17" s="4"/>
       <c r="BK17" s="4"/>
-      <c r="BL17" s="6"/>
+      <c r="BL17" s="4"/>
       <c r="BM17" s="6"/>
       <c r="BN17" s="6"/>
       <c r="BO17" s="6"/>
-    </row>
-    <row r="18" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP17" s="6"/>
+    </row>
+    <row r="18" customFormat="false" ht="162" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="n">
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="5" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
@@ -1925,24 +1994,25 @@
       <c r="BI18" s="4"/>
       <c r="BJ18" s="4"/>
       <c r="BK18" s="4"/>
-      <c r="BL18" s="6"/>
+      <c r="BL18" s="4"/>
       <c r="BM18" s="6"/>
       <c r="BN18" s="6"/>
       <c r="BO18" s="6"/>
-    </row>
-    <row r="19" customFormat="false" ht="359.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP18" s="6"/>
+    </row>
+    <row r="19" customFormat="false" ht="359.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="n">
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="5" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
@@ -2002,24 +2072,25 @@
       <c r="BI19" s="4"/>
       <c r="BJ19" s="4"/>
       <c r="BK19" s="4"/>
-      <c r="BL19" s="6"/>
+      <c r="BL19" s="4"/>
       <c r="BM19" s="6"/>
       <c r="BN19" s="6"/>
       <c r="BO19" s="6"/>
-    </row>
-    <row r="20" customFormat="false" ht="61.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="BP19" s="6"/>
+    </row>
+    <row r="20" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="n">
         <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="5" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
@@ -2079,24 +2150,25 @@
       <c r="BI20" s="4"/>
       <c r="BJ20" s="4"/>
       <c r="BK20" s="4"/>
-      <c r="BL20" s="6"/>
+      <c r="BL20" s="4"/>
       <c r="BM20" s="6"/>
       <c r="BN20" s="6"/>
       <c r="BO20" s="6"/>
-    </row>
-    <row r="21" customFormat="false" ht="126.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP20" s="6"/>
+    </row>
+    <row r="21" customFormat="false" ht="126.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="n">
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="5" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
@@ -2156,12 +2228,13 @@
       <c r="BI21" s="4"/>
       <c r="BJ21" s="4"/>
       <c r="BK21" s="4"/>
-      <c r="BL21" s="6"/>
+      <c r="BL21" s="4"/>
       <c r="BM21" s="6"/>
       <c r="BN21" s="6"/>
       <c r="BO21" s="6"/>
-    </row>
-    <row r="22" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP21" s="6"/>
+    </row>
+    <row r="22" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -2225,22 +2298,23 @@
       <c r="BI22" s="4"/>
       <c r="BJ22" s="4"/>
       <c r="BK22" s="4"/>
-      <c r="BL22" s="6"/>
+      <c r="BL22" s="4"/>
       <c r="BM22" s="6"/>
       <c r="BN22" s="6"/>
       <c r="BO22" s="6"/>
-    </row>
-    <row r="23" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP22" s="6"/>
+    </row>
+    <row r="23" customFormat="false" ht="135.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="4"/>
       <c r="B23" s="4" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="7" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
@@ -2300,15 +2374,16 @@
       <c r="BI23" s="4"/>
       <c r="BJ23" s="4"/>
       <c r="BK23" s="4"/>
-      <c r="BL23" s="6"/>
+      <c r="BL23" s="4"/>
       <c r="BM23" s="6"/>
       <c r="BN23" s="6"/>
       <c r="BO23" s="6"/>
-    </row>
-    <row r="24" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP23" s="6"/>
+    </row>
+    <row r="24" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="4"/>
       <c r="B24" s="4" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -2371,15 +2446,16 @@
       <c r="BI24" s="4"/>
       <c r="BJ24" s="4"/>
       <c r="BK24" s="4"/>
-      <c r="BL24" s="6"/>
+      <c r="BL24" s="4"/>
       <c r="BM24" s="6"/>
       <c r="BN24" s="6"/>
       <c r="BO24" s="6"/>
-    </row>
-    <row r="25" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP24" s="6"/>
+    </row>
+    <row r="25" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="4"/>
       <c r="B25" s="4" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -2442,15 +2518,16 @@
       <c r="BI25" s="4"/>
       <c r="BJ25" s="4"/>
       <c r="BK25" s="4"/>
-      <c r="BL25" s="6"/>
+      <c r="BL25" s="4"/>
       <c r="BM25" s="6"/>
       <c r="BN25" s="6"/>
       <c r="BO25" s="6"/>
-    </row>
-    <row r="26" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP25" s="6"/>
+    </row>
+    <row r="26" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="4"/>
       <c r="B26" s="4" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
@@ -2513,15 +2590,16 @@
       <c r="BI26" s="4"/>
       <c r="BJ26" s="4"/>
       <c r="BK26" s="4"/>
-      <c r="BL26" s="6"/>
+      <c r="BL26" s="4"/>
       <c r="BM26" s="6"/>
       <c r="BN26" s="6"/>
       <c r="BO26" s="6"/>
-    </row>
-    <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP26" s="6"/>
+    </row>
+    <row r="27" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="4"/>
       <c r="B27" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
@@ -2584,12 +2662,13 @@
       <c r="BI27" s="4"/>
       <c r="BJ27" s="4"/>
       <c r="BK27" s="4"/>
-      <c r="BL27" s="6"/>
+      <c r="BL27" s="4"/>
       <c r="BM27" s="6"/>
       <c r="BN27" s="6"/>
       <c r="BO27" s="6"/>
-    </row>
-    <row r="28" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP27" s="6"/>
+    </row>
+    <row r="28" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -2653,12 +2732,13 @@
       <c r="BI28" s="4"/>
       <c r="BJ28" s="4"/>
       <c r="BK28" s="4"/>
-      <c r="BL28" s="6"/>
+      <c r="BL28" s="4"/>
       <c r="BM28" s="6"/>
       <c r="BN28" s="6"/>
       <c r="BO28" s="6"/>
-    </row>
-    <row r="29" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP28" s="6"/>
+    </row>
+    <row r="29" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -2722,12 +2802,13 @@
       <c r="BI29" s="4"/>
       <c r="BJ29" s="4"/>
       <c r="BK29" s="4"/>
-      <c r="BL29" s="6"/>
+      <c r="BL29" s="4"/>
       <c r="BM29" s="6"/>
       <c r="BN29" s="6"/>
       <c r="BO29" s="6"/>
-    </row>
-    <row r="30" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP29" s="6"/>
+    </row>
+    <row r="30" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -2791,12 +2872,13 @@
       <c r="BI30" s="4"/>
       <c r="BJ30" s="4"/>
       <c r="BK30" s="4"/>
-      <c r="BL30" s="6"/>
+      <c r="BL30" s="4"/>
       <c r="BM30" s="6"/>
       <c r="BN30" s="6"/>
       <c r="BO30" s="6"/>
-    </row>
-    <row r="31" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP30" s="6"/>
+    </row>
+    <row r="31" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -2860,12 +2942,13 @@
       <c r="BI31" s="4"/>
       <c r="BJ31" s="4"/>
       <c r="BK31" s="4"/>
-      <c r="BL31" s="6"/>
+      <c r="BL31" s="4"/>
       <c r="BM31" s="6"/>
       <c r="BN31" s="6"/>
       <c r="BO31" s="6"/>
-    </row>
-    <row r="32" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP31" s="6"/>
+    </row>
+    <row r="32" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -2929,12 +3012,13 @@
       <c r="BI32" s="4"/>
       <c r="BJ32" s="4"/>
       <c r="BK32" s="4"/>
-      <c r="BL32" s="6"/>
+      <c r="BL32" s="4"/>
       <c r="BM32" s="6"/>
       <c r="BN32" s="6"/>
       <c r="BO32" s="6"/>
-    </row>
-    <row r="33" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP32" s="6"/>
+    </row>
+    <row r="33" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -2998,12 +3082,13 @@
       <c r="BI33" s="4"/>
       <c r="BJ33" s="4"/>
       <c r="BK33" s="4"/>
-      <c r="BL33" s="6"/>
+      <c r="BL33" s="4"/>
       <c r="BM33" s="6"/>
       <c r="BN33" s="6"/>
       <c r="BO33" s="6"/>
-    </row>
-    <row r="34" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP33" s="6"/>
+    </row>
+    <row r="34" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -3067,12 +3152,13 @@
       <c r="BI34" s="4"/>
       <c r="BJ34" s="4"/>
       <c r="BK34" s="4"/>
-      <c r="BL34" s="6"/>
+      <c r="BL34" s="4"/>
       <c r="BM34" s="6"/>
       <c r="BN34" s="6"/>
       <c r="BO34" s="6"/>
-    </row>
-    <row r="35" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP34" s="6"/>
+    </row>
+    <row r="35" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -3136,12 +3222,13 @@
       <c r="BI35" s="4"/>
       <c r="BJ35" s="4"/>
       <c r="BK35" s="4"/>
-      <c r="BL35" s="6"/>
+      <c r="BL35" s="4"/>
       <c r="BM35" s="6"/>
       <c r="BN35" s="6"/>
       <c r="BO35" s="6"/>
-    </row>
-    <row r="36" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP35" s="6"/>
+    </row>
+    <row r="36" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -3205,12 +3292,13 @@
       <c r="BI36" s="4"/>
       <c r="BJ36" s="4"/>
       <c r="BK36" s="4"/>
-      <c r="BL36" s="6"/>
+      <c r="BL36" s="4"/>
       <c r="BM36" s="6"/>
       <c r="BN36" s="6"/>
       <c r="BO36" s="6"/>
-    </row>
-    <row r="37" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP36" s="6"/>
+    </row>
+    <row r="37" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -3274,12 +3362,13 @@
       <c r="BI37" s="4"/>
       <c r="BJ37" s="4"/>
       <c r="BK37" s="4"/>
-      <c r="BL37" s="6"/>
+      <c r="BL37" s="4"/>
       <c r="BM37" s="6"/>
       <c r="BN37" s="6"/>
       <c r="BO37" s="6"/>
-    </row>
-    <row r="38" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP37" s="6"/>
+    </row>
+    <row r="38" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -3343,12 +3432,13 @@
       <c r="BI38" s="4"/>
       <c r="BJ38" s="4"/>
       <c r="BK38" s="4"/>
-      <c r="BL38" s="6"/>
+      <c r="BL38" s="4"/>
       <c r="BM38" s="6"/>
       <c r="BN38" s="6"/>
       <c r="BO38" s="6"/>
-    </row>
-    <row r="39" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP38" s="6"/>
+    </row>
+    <row r="39" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -3412,12 +3502,13 @@
       <c r="BI39" s="4"/>
       <c r="BJ39" s="4"/>
       <c r="BK39" s="4"/>
-      <c r="BL39" s="6"/>
+      <c r="BL39" s="4"/>
       <c r="BM39" s="6"/>
       <c r="BN39" s="6"/>
       <c r="BO39" s="6"/>
-    </row>
-    <row r="40" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP39" s="6"/>
+    </row>
+    <row r="40" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -3481,12 +3572,13 @@
       <c r="BI40" s="4"/>
       <c r="BJ40" s="4"/>
       <c r="BK40" s="4"/>
-      <c r="BL40" s="6"/>
+      <c r="BL40" s="4"/>
       <c r="BM40" s="6"/>
       <c r="BN40" s="6"/>
       <c r="BO40" s="6"/>
-    </row>
-    <row r="41" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP40" s="6"/>
+    </row>
+    <row r="41" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -3550,12 +3642,13 @@
       <c r="BI41" s="4"/>
       <c r="BJ41" s="4"/>
       <c r="BK41" s="4"/>
-      <c r="BL41" s="6"/>
+      <c r="BL41" s="4"/>
       <c r="BM41" s="6"/>
       <c r="BN41" s="6"/>
       <c r="BO41" s="6"/>
-    </row>
-    <row r="42" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP41" s="6"/>
+    </row>
+    <row r="42" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -3619,12 +3712,13 @@
       <c r="BI42" s="4"/>
       <c r="BJ42" s="4"/>
       <c r="BK42" s="4"/>
-      <c r="BL42" s="6"/>
+      <c r="BL42" s="4"/>
       <c r="BM42" s="6"/>
       <c r="BN42" s="6"/>
       <c r="BO42" s="6"/>
-    </row>
-    <row r="43" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP42" s="6"/>
+    </row>
+    <row r="43" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -3688,12 +3782,13 @@
       <c r="BI43" s="4"/>
       <c r="BJ43" s="4"/>
       <c r="BK43" s="4"/>
-      <c r="BL43" s="6"/>
+      <c r="BL43" s="4"/>
       <c r="BM43" s="6"/>
       <c r="BN43" s="6"/>
       <c r="BO43" s="6"/>
-    </row>
-    <row r="44" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP43" s="6"/>
+    </row>
+    <row r="44" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
@@ -3757,12 +3852,13 @@
       <c r="BI44" s="4"/>
       <c r="BJ44" s="4"/>
       <c r="BK44" s="4"/>
-      <c r="BL44" s="6"/>
+      <c r="BL44" s="4"/>
       <c r="BM44" s="6"/>
       <c r="BN44" s="6"/>
       <c r="BO44" s="6"/>
-    </row>
-    <row r="45" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP44" s="6"/>
+    </row>
+    <row r="45" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
@@ -3826,12 +3922,13 @@
       <c r="BI45" s="4"/>
       <c r="BJ45" s="4"/>
       <c r="BK45" s="4"/>
-      <c r="BL45" s="6"/>
+      <c r="BL45" s="4"/>
       <c r="BM45" s="6"/>
       <c r="BN45" s="6"/>
       <c r="BO45" s="6"/>
-    </row>
-    <row r="46" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP45" s="6"/>
+    </row>
+    <row r="46" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
@@ -3895,12 +3992,13 @@
       <c r="BI46" s="4"/>
       <c r="BJ46" s="4"/>
       <c r="BK46" s="4"/>
-      <c r="BL46" s="6"/>
+      <c r="BL46" s="4"/>
       <c r="BM46" s="6"/>
       <c r="BN46" s="6"/>
       <c r="BO46" s="6"/>
-    </row>
-    <row r="47" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP46" s="6"/>
+    </row>
+    <row r="47" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -3964,12 +4062,13 @@
       <c r="BI47" s="4"/>
       <c r="BJ47" s="4"/>
       <c r="BK47" s="4"/>
-      <c r="BL47" s="6"/>
+      <c r="BL47" s="4"/>
       <c r="BM47" s="6"/>
       <c r="BN47" s="6"/>
       <c r="BO47" s="6"/>
-    </row>
-    <row r="48" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP47" s="6"/>
+    </row>
+    <row r="48" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
@@ -4033,12 +4132,13 @@
       <c r="BI48" s="4"/>
       <c r="BJ48" s="4"/>
       <c r="BK48" s="4"/>
-      <c r="BL48" s="6"/>
+      <c r="BL48" s="4"/>
       <c r="BM48" s="6"/>
       <c r="BN48" s="6"/>
       <c r="BO48" s="6"/>
-    </row>
-    <row r="49" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP48" s="6"/>
+    </row>
+    <row r="49" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="4"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
@@ -4102,12 +4202,13 @@
       <c r="BI49" s="4"/>
       <c r="BJ49" s="4"/>
       <c r="BK49" s="4"/>
-      <c r="BL49" s="6"/>
+      <c r="BL49" s="4"/>
       <c r="BM49" s="6"/>
       <c r="BN49" s="6"/>
       <c r="BO49" s="6"/>
-    </row>
-    <row r="50" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP49" s="6"/>
+    </row>
+    <row r="50" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
@@ -4171,12 +4272,13 @@
       <c r="BI50" s="4"/>
       <c r="BJ50" s="4"/>
       <c r="BK50" s="4"/>
-      <c r="BL50" s="6"/>
+      <c r="BL50" s="4"/>
       <c r="BM50" s="6"/>
       <c r="BN50" s="6"/>
       <c r="BO50" s="6"/>
-    </row>
-    <row r="51" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP50" s="6"/>
+    </row>
+    <row r="51" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
@@ -4240,12 +4342,13 @@
       <c r="BI51" s="4"/>
       <c r="BJ51" s="4"/>
       <c r="BK51" s="4"/>
-      <c r="BL51" s="6"/>
+      <c r="BL51" s="4"/>
       <c r="BM51" s="6"/>
       <c r="BN51" s="6"/>
       <c r="BO51" s="6"/>
-    </row>
-    <row r="52" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP51" s="6"/>
+    </row>
+    <row r="52" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
@@ -4309,12 +4412,13 @@
       <c r="BI52" s="4"/>
       <c r="BJ52" s="4"/>
       <c r="BK52" s="4"/>
-      <c r="BL52" s="6"/>
+      <c r="BL52" s="4"/>
       <c r="BM52" s="6"/>
       <c r="BN52" s="6"/>
       <c r="BO52" s="6"/>
-    </row>
-    <row r="53" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP52" s="6"/>
+    </row>
+    <row r="53" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="4"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
@@ -4378,12 +4482,13 @@
       <c r="BI53" s="4"/>
       <c r="BJ53" s="4"/>
       <c r="BK53" s="4"/>
-      <c r="BL53" s="6"/>
+      <c r="BL53" s="4"/>
       <c r="BM53" s="6"/>
       <c r="BN53" s="6"/>
       <c r="BO53" s="6"/>
-    </row>
-    <row r="54" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP53" s="6"/>
+    </row>
+    <row r="54" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="4"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
@@ -4447,12 +4552,13 @@
       <c r="BI54" s="4"/>
       <c r="BJ54" s="4"/>
       <c r="BK54" s="4"/>
-      <c r="BL54" s="6"/>
+      <c r="BL54" s="4"/>
       <c r="BM54" s="6"/>
       <c r="BN54" s="6"/>
       <c r="BO54" s="6"/>
-    </row>
-    <row r="55" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP54" s="6"/>
+    </row>
+    <row r="55" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="4"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
@@ -4516,12 +4622,13 @@
       <c r="BI55" s="4"/>
       <c r="BJ55" s="4"/>
       <c r="BK55" s="4"/>
-      <c r="BL55" s="6"/>
+      <c r="BL55" s="4"/>
       <c r="BM55" s="6"/>
       <c r="BN55" s="6"/>
       <c r="BO55" s="6"/>
-    </row>
-    <row r="56" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP55" s="6"/>
+    </row>
+    <row r="56" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="4"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
@@ -4585,12 +4692,13 @@
       <c r="BI56" s="4"/>
       <c r="BJ56" s="4"/>
       <c r="BK56" s="4"/>
-      <c r="BL56" s="6"/>
+      <c r="BL56" s="4"/>
       <c r="BM56" s="6"/>
       <c r="BN56" s="6"/>
       <c r="BO56" s="6"/>
-    </row>
-    <row r="57" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP56" s="6"/>
+    </row>
+    <row r="57" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="4"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
@@ -4654,12 +4762,13 @@
       <c r="BI57" s="4"/>
       <c r="BJ57" s="4"/>
       <c r="BK57" s="4"/>
-      <c r="BL57" s="6"/>
+      <c r="BL57" s="4"/>
       <c r="BM57" s="6"/>
       <c r="BN57" s="6"/>
       <c r="BO57" s="6"/>
-    </row>
-    <row r="58" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP57" s="6"/>
+    </row>
+    <row r="58" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
@@ -4723,12 +4832,13 @@
       <c r="BI58" s="4"/>
       <c r="BJ58" s="4"/>
       <c r="BK58" s="4"/>
-      <c r="BL58" s="6"/>
+      <c r="BL58" s="4"/>
       <c r="BM58" s="6"/>
       <c r="BN58" s="6"/>
       <c r="BO58" s="6"/>
-    </row>
-    <row r="59" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP58" s="6"/>
+    </row>
+    <row r="59" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="4"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
@@ -4792,12 +4902,13 @@
       <c r="BI59" s="4"/>
       <c r="BJ59" s="4"/>
       <c r="BK59" s="4"/>
-      <c r="BL59" s="6"/>
+      <c r="BL59" s="4"/>
       <c r="BM59" s="6"/>
       <c r="BN59" s="6"/>
       <c r="BO59" s="6"/>
-    </row>
-    <row r="60" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP59" s="6"/>
+    </row>
+    <row r="60" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
@@ -4861,12 +4972,13 @@
       <c r="BI60" s="4"/>
       <c r="BJ60" s="4"/>
       <c r="BK60" s="4"/>
-      <c r="BL60" s="6"/>
+      <c r="BL60" s="4"/>
       <c r="BM60" s="6"/>
       <c r="BN60" s="6"/>
       <c r="BO60" s="6"/>
-    </row>
-    <row r="61" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP60" s="6"/>
+    </row>
+    <row r="61" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="4"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
@@ -4930,12 +5042,13 @@
       <c r="BI61" s="4"/>
       <c r="BJ61" s="4"/>
       <c r="BK61" s="4"/>
-      <c r="BL61" s="6"/>
+      <c r="BL61" s="4"/>
       <c r="BM61" s="6"/>
       <c r="BN61" s="6"/>
       <c r="BO61" s="6"/>
-    </row>
-    <row r="62" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP61" s="6"/>
+    </row>
+    <row r="62" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="4"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
@@ -4999,12 +5112,13 @@
       <c r="BI62" s="4"/>
       <c r="BJ62" s="4"/>
       <c r="BK62" s="4"/>
-      <c r="BL62" s="6"/>
+      <c r="BL62" s="4"/>
       <c r="BM62" s="6"/>
       <c r="BN62" s="6"/>
       <c r="BO62" s="6"/>
-    </row>
-    <row r="63" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP62" s="6"/>
+    </row>
+    <row r="63" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="4"/>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
@@ -5068,12 +5182,13 @@
       <c r="BI63" s="4"/>
       <c r="BJ63" s="4"/>
       <c r="BK63" s="4"/>
-      <c r="BL63" s="6"/>
+      <c r="BL63" s="4"/>
       <c r="BM63" s="6"/>
       <c r="BN63" s="6"/>
       <c r="BO63" s="6"/>
-    </row>
-    <row r="64" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP63" s="6"/>
+    </row>
+    <row r="64" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="4"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
@@ -5137,12 +5252,13 @@
       <c r="BI64" s="4"/>
       <c r="BJ64" s="4"/>
       <c r="BK64" s="4"/>
-      <c r="BL64" s="6"/>
+      <c r="BL64" s="4"/>
       <c r="BM64" s="6"/>
       <c r="BN64" s="6"/>
       <c r="BO64" s="6"/>
-    </row>
-    <row r="65" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP64" s="6"/>
+    </row>
+    <row r="65" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="4"/>
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
@@ -5206,12 +5322,13 @@
       <c r="BI65" s="4"/>
       <c r="BJ65" s="4"/>
       <c r="BK65" s="4"/>
-      <c r="BL65" s="6"/>
+      <c r="BL65" s="4"/>
       <c r="BM65" s="6"/>
       <c r="BN65" s="6"/>
       <c r="BO65" s="6"/>
-    </row>
-    <row r="66" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP65" s="6"/>
+    </row>
+    <row r="66" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="4"/>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
@@ -5275,12 +5392,13 @@
       <c r="BI66" s="4"/>
       <c r="BJ66" s="4"/>
       <c r="BK66" s="4"/>
-      <c r="BL66" s="6"/>
+      <c r="BL66" s="4"/>
       <c r="BM66" s="6"/>
       <c r="BN66" s="6"/>
       <c r="BO66" s="6"/>
-    </row>
-    <row r="67" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP66" s="6"/>
+    </row>
+    <row r="67" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="4"/>
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
@@ -5344,12 +5462,13 @@
       <c r="BI67" s="4"/>
       <c r="BJ67" s="4"/>
       <c r="BK67" s="4"/>
-      <c r="BL67" s="6"/>
+      <c r="BL67" s="4"/>
       <c r="BM67" s="6"/>
       <c r="BN67" s="6"/>
       <c r="BO67" s="6"/>
-    </row>
-    <row r="68" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP67" s="6"/>
+    </row>
+    <row r="68" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="4"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
@@ -5413,12 +5532,13 @@
       <c r="BI68" s="4"/>
       <c r="BJ68" s="4"/>
       <c r="BK68" s="4"/>
-      <c r="BL68" s="6"/>
+      <c r="BL68" s="4"/>
       <c r="BM68" s="6"/>
       <c r="BN68" s="6"/>
       <c r="BO68" s="6"/>
-    </row>
-    <row r="69" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP68" s="6"/>
+    </row>
+    <row r="69" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="4"/>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
@@ -5482,12 +5602,13 @@
       <c r="BI69" s="4"/>
       <c r="BJ69" s="4"/>
       <c r="BK69" s="4"/>
-      <c r="BL69" s="6"/>
+      <c r="BL69" s="4"/>
       <c r="BM69" s="6"/>
       <c r="BN69" s="6"/>
       <c r="BO69" s="6"/>
-    </row>
-    <row r="70" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP69" s="6"/>
+    </row>
+    <row r="70" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
@@ -5551,12 +5672,13 @@
       <c r="BI70" s="4"/>
       <c r="BJ70" s="4"/>
       <c r="BK70" s="4"/>
-      <c r="BL70" s="6"/>
+      <c r="BL70" s="4"/>
       <c r="BM70" s="6"/>
       <c r="BN70" s="6"/>
       <c r="BO70" s="6"/>
-    </row>
-    <row r="71" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP70" s="6"/>
+    </row>
+    <row r="71" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
@@ -5620,12 +5742,13 @@
       <c r="BI71" s="4"/>
       <c r="BJ71" s="4"/>
       <c r="BK71" s="4"/>
-      <c r="BL71" s="6"/>
+      <c r="BL71" s="4"/>
       <c r="BM71" s="6"/>
       <c r="BN71" s="6"/>
       <c r="BO71" s="6"/>
-    </row>
-    <row r="72" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP71" s="6"/>
+    </row>
+    <row r="72" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="4"/>
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
@@ -5689,12 +5812,13 @@
       <c r="BI72" s="4"/>
       <c r="BJ72" s="4"/>
       <c r="BK72" s="4"/>
-      <c r="BL72" s="6"/>
+      <c r="BL72" s="4"/>
       <c r="BM72" s="6"/>
       <c r="BN72" s="6"/>
       <c r="BO72" s="6"/>
-    </row>
-    <row r="73" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP72" s="6"/>
+    </row>
+    <row r="73" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
@@ -5758,12 +5882,13 @@
       <c r="BI73" s="4"/>
       <c r="BJ73" s="4"/>
       <c r="BK73" s="4"/>
-      <c r="BL73" s="6"/>
+      <c r="BL73" s="4"/>
       <c r="BM73" s="6"/>
       <c r="BN73" s="6"/>
       <c r="BO73" s="6"/>
-    </row>
-    <row r="74" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP73" s="6"/>
+    </row>
+    <row r="74" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="4"/>
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
@@ -5827,12 +5952,13 @@
       <c r="BI74" s="4"/>
       <c r="BJ74" s="4"/>
       <c r="BK74" s="4"/>
-      <c r="BL74" s="6"/>
+      <c r="BL74" s="4"/>
       <c r="BM74" s="6"/>
       <c r="BN74" s="6"/>
       <c r="BO74" s="6"/>
-    </row>
-    <row r="75" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP74" s="6"/>
+    </row>
+    <row r="75" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="4"/>
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
@@ -5896,12 +6022,13 @@
       <c r="BI75" s="4"/>
       <c r="BJ75" s="4"/>
       <c r="BK75" s="4"/>
-      <c r="BL75" s="6"/>
+      <c r="BL75" s="4"/>
       <c r="BM75" s="6"/>
       <c r="BN75" s="6"/>
       <c r="BO75" s="6"/>
-    </row>
-    <row r="76" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP75" s="6"/>
+    </row>
+    <row r="76" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="4"/>
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
@@ -5965,12 +6092,13 @@
       <c r="BI76" s="4"/>
       <c r="BJ76" s="4"/>
       <c r="BK76" s="4"/>
-      <c r="BL76" s="6"/>
+      <c r="BL76" s="4"/>
       <c r="BM76" s="6"/>
       <c r="BN76" s="6"/>
       <c r="BO76" s="6"/>
-    </row>
-    <row r="77" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP76" s="6"/>
+    </row>
+    <row r="77" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="4"/>
       <c r="B77" s="4"/>
       <c r="C77" s="4"/>
@@ -6034,12 +6162,13 @@
       <c r="BI77" s="4"/>
       <c r="BJ77" s="4"/>
       <c r="BK77" s="4"/>
-      <c r="BL77" s="6"/>
+      <c r="BL77" s="4"/>
       <c r="BM77" s="6"/>
       <c r="BN77" s="6"/>
       <c r="BO77" s="6"/>
-    </row>
-    <row r="78" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP77" s="6"/>
+    </row>
+    <row r="78" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="4"/>
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
@@ -6103,12 +6232,13 @@
       <c r="BI78" s="4"/>
       <c r="BJ78" s="4"/>
       <c r="BK78" s="4"/>
-      <c r="BL78" s="6"/>
+      <c r="BL78" s="4"/>
       <c r="BM78" s="6"/>
       <c r="BN78" s="6"/>
       <c r="BO78" s="6"/>
-    </row>
-    <row r="79" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP78" s="6"/>
+    </row>
+    <row r="79" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="4"/>
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
@@ -6172,12 +6302,13 @@
       <c r="BI79" s="4"/>
       <c r="BJ79" s="4"/>
       <c r="BK79" s="4"/>
-      <c r="BL79" s="6"/>
+      <c r="BL79" s="4"/>
       <c r="BM79" s="6"/>
       <c r="BN79" s="6"/>
       <c r="BO79" s="6"/>
-    </row>
-    <row r="80" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP79" s="6"/>
+    </row>
+    <row r="80" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="4"/>
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
@@ -6241,12 +6372,13 @@
       <c r="BI80" s="4"/>
       <c r="BJ80" s="4"/>
       <c r="BK80" s="4"/>
-      <c r="BL80" s="6"/>
+      <c r="BL80" s="4"/>
       <c r="BM80" s="6"/>
       <c r="BN80" s="6"/>
       <c r="BO80" s="6"/>
-    </row>
-    <row r="81" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP80" s="6"/>
+    </row>
+    <row r="81" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="4"/>
       <c r="B81" s="4"/>
       <c r="C81" s="4"/>
@@ -6310,12 +6442,13 @@
       <c r="BI81" s="4"/>
       <c r="BJ81" s="4"/>
       <c r="BK81" s="4"/>
-      <c r="BL81" s="6"/>
+      <c r="BL81" s="4"/>
       <c r="BM81" s="6"/>
       <c r="BN81" s="6"/>
       <c r="BO81" s="6"/>
-    </row>
-    <row r="82" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP81" s="6"/>
+    </row>
+    <row r="82" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="4"/>
       <c r="B82" s="4"/>
       <c r="C82" s="4"/>
@@ -6379,12 +6512,13 @@
       <c r="BI82" s="4"/>
       <c r="BJ82" s="4"/>
       <c r="BK82" s="4"/>
-      <c r="BL82" s="6"/>
+      <c r="BL82" s="4"/>
       <c r="BM82" s="6"/>
       <c r="BN82" s="6"/>
       <c r="BO82" s="6"/>
-    </row>
-    <row r="83" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP82" s="6"/>
+    </row>
+    <row r="83" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="4"/>
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
@@ -6448,12 +6582,13 @@
       <c r="BI83" s="4"/>
       <c r="BJ83" s="4"/>
       <c r="BK83" s="4"/>
-      <c r="BL83" s="6"/>
+      <c r="BL83" s="4"/>
       <c r="BM83" s="6"/>
       <c r="BN83" s="6"/>
       <c r="BO83" s="6"/>
-    </row>
-    <row r="84" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP83" s="6"/>
+    </row>
+    <row r="84" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="4"/>
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
@@ -6517,12 +6652,13 @@
       <c r="BI84" s="4"/>
       <c r="BJ84" s="4"/>
       <c r="BK84" s="4"/>
-      <c r="BL84" s="6"/>
+      <c r="BL84" s="4"/>
       <c r="BM84" s="6"/>
       <c r="BN84" s="6"/>
       <c r="BO84" s="6"/>
-    </row>
-    <row r="85" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP84" s="6"/>
+    </row>
+    <row r="85" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="4"/>
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
@@ -6586,12 +6722,13 @@
       <c r="BI85" s="4"/>
       <c r="BJ85" s="4"/>
       <c r="BK85" s="4"/>
-      <c r="BL85" s="6"/>
+      <c r="BL85" s="4"/>
       <c r="BM85" s="6"/>
       <c r="BN85" s="6"/>
       <c r="BO85" s="6"/>
-    </row>
-    <row r="86" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP85" s="6"/>
+    </row>
+    <row r="86" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="4"/>
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
@@ -6655,12 +6792,13 @@
       <c r="BI86" s="4"/>
       <c r="BJ86" s="4"/>
       <c r="BK86" s="4"/>
-      <c r="BL86" s="6"/>
+      <c r="BL86" s="4"/>
       <c r="BM86" s="6"/>
       <c r="BN86" s="6"/>
       <c r="BO86" s="6"/>
-    </row>
-    <row r="87" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP86" s="6"/>
+    </row>
+    <row r="87" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="4"/>
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
@@ -6724,12 +6862,13 @@
       <c r="BI87" s="4"/>
       <c r="BJ87" s="4"/>
       <c r="BK87" s="4"/>
-      <c r="BL87" s="6"/>
+      <c r="BL87" s="4"/>
       <c r="BM87" s="6"/>
       <c r="BN87" s="6"/>
       <c r="BO87" s="6"/>
-    </row>
-    <row r="88" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP87" s="6"/>
+    </row>
+    <row r="88" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="4"/>
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
@@ -6793,12 +6932,13 @@
       <c r="BI88" s="4"/>
       <c r="BJ88" s="4"/>
       <c r="BK88" s="4"/>
-      <c r="BL88" s="6"/>
+      <c r="BL88" s="4"/>
       <c r="BM88" s="6"/>
       <c r="BN88" s="6"/>
       <c r="BO88" s="6"/>
-    </row>
-    <row r="89" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP88" s="6"/>
+    </row>
+    <row r="89" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="4"/>
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
@@ -6862,12 +7002,13 @@
       <c r="BI89" s="4"/>
       <c r="BJ89" s="4"/>
       <c r="BK89" s="4"/>
-      <c r="BL89" s="6"/>
+      <c r="BL89" s="4"/>
       <c r="BM89" s="6"/>
       <c r="BN89" s="6"/>
       <c r="BO89" s="6"/>
-    </row>
-    <row r="90" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP89" s="6"/>
+    </row>
+    <row r="90" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="4"/>
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
@@ -6931,12 +7072,13 @@
       <c r="BI90" s="4"/>
       <c r="BJ90" s="4"/>
       <c r="BK90" s="4"/>
-      <c r="BL90" s="6"/>
+      <c r="BL90" s="4"/>
       <c r="BM90" s="6"/>
       <c r="BN90" s="6"/>
       <c r="BO90" s="6"/>
-    </row>
-    <row r="91" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP90" s="6"/>
+    </row>
+    <row r="91" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="4"/>
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
@@ -7000,12 +7142,13 @@
       <c r="BI91" s="4"/>
       <c r="BJ91" s="4"/>
       <c r="BK91" s="4"/>
-      <c r="BL91" s="6"/>
+      <c r="BL91" s="4"/>
       <c r="BM91" s="6"/>
       <c r="BN91" s="6"/>
       <c r="BO91" s="6"/>
-    </row>
-    <row r="92" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP91" s="6"/>
+    </row>
+    <row r="92" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="4"/>
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
@@ -7069,12 +7212,13 @@
       <c r="BI92" s="4"/>
       <c r="BJ92" s="4"/>
       <c r="BK92" s="4"/>
-      <c r="BL92" s="6"/>
+      <c r="BL92" s="4"/>
       <c r="BM92" s="6"/>
       <c r="BN92" s="6"/>
       <c r="BO92" s="6"/>
-    </row>
-    <row r="93" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BP92" s="6"/>
+    </row>
+    <row r="93" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="4"/>
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
@@ -7138,8 +7282,9 @@
       <c r="BI93" s="4"/>
       <c r="BJ93" s="4"/>
       <c r="BK93" s="4"/>
-    </row>
-    <row r="94" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BL93" s="4"/>
+    </row>
+    <row r="94" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="4"/>
       <c r="B94" s="4"/>
       <c r="C94" s="4"/>
@@ -7203,8 +7348,9 @@
       <c r="BI94" s="4"/>
       <c r="BJ94" s="4"/>
       <c r="BK94" s="4"/>
-    </row>
-    <row r="95" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BL94" s="4"/>
+    </row>
+    <row r="95" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="4"/>
       <c r="B95" s="4"/>
       <c r="C95" s="4"/>
@@ -7268,8 +7414,9 @@
       <c r="BI95" s="4"/>
       <c r="BJ95" s="4"/>
       <c r="BK95" s="4"/>
-    </row>
-    <row r="96" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BL95" s="4"/>
+    </row>
+    <row r="96" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="4"/>
       <c r="B96" s="4"/>
       <c r="C96" s="4"/>
@@ -7333,8 +7480,9 @@
       <c r="BI96" s="4"/>
       <c r="BJ96" s="4"/>
       <c r="BK96" s="4"/>
-    </row>
-    <row r="97" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BL96" s="4"/>
+    </row>
+    <row r="97" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="4"/>
       <c r="B97" s="4"/>
       <c r="C97" s="4"/>
@@ -7398,8 +7546,9 @@
       <c r="BI97" s="4"/>
       <c r="BJ97" s="4"/>
       <c r="BK97" s="4"/>
-    </row>
-    <row r="98" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BL97" s="4"/>
+    </row>
+    <row r="98" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="4"/>
       <c r="B98" s="4"/>
       <c r="C98" s="4"/>
@@ -7463,8 +7612,9 @@
       <c r="BI98" s="4"/>
       <c r="BJ98" s="4"/>
       <c r="BK98" s="4"/>
-    </row>
-    <row r="99" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BL98" s="4"/>
+    </row>
+    <row r="99" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="4"/>
       <c r="B99" s="4"/>
       <c r="C99" s="4"/>
@@ -7528,8 +7678,9 @@
       <c r="BI99" s="4"/>
       <c r="BJ99" s="4"/>
       <c r="BK99" s="4"/>
-    </row>
-    <row r="100" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BL99" s="4"/>
+    </row>
+    <row r="100" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="4"/>
       <c r="B100" s="4"/>
       <c r="C100" s="4"/>
@@ -7593,8 +7744,9 @@
       <c r="BI100" s="4"/>
       <c r="BJ100" s="4"/>
       <c r="BK100" s="4"/>
-    </row>
-    <row r="101" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BL100" s="4"/>
+    </row>
+    <row r="101" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="4"/>
       <c r="B101" s="4"/>
       <c r="C101" s="4"/>
@@ -7658,8 +7810,9 @@
       <c r="BI101" s="4"/>
       <c r="BJ101" s="4"/>
       <c r="BK101" s="4"/>
-    </row>
-    <row r="102" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BL101" s="4"/>
+    </row>
+    <row r="102" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="4"/>
       <c r="B102" s="4"/>
       <c r="C102" s="4"/>
@@ -7723,8 +7876,9 @@
       <c r="BI102" s="4"/>
       <c r="BJ102" s="4"/>
       <c r="BK102" s="4"/>
-    </row>
-    <row r="103" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BL102" s="4"/>
+    </row>
+    <row r="103" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="4"/>
       <c r="B103" s="4"/>
       <c r="C103" s="4"/>
@@ -7788,8 +7942,9 @@
       <c r="BI103" s="4"/>
       <c r="BJ103" s="4"/>
       <c r="BK103" s="4"/>
-    </row>
-    <row r="104" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BL103" s="4"/>
+    </row>
+    <row r="104" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="4"/>
       <c r="B104" s="4"/>
       <c r="C104" s="4"/>
@@ -7853,8 +8008,9 @@
       <c r="BI104" s="4"/>
       <c r="BJ104" s="4"/>
       <c r="BK104" s="4"/>
-    </row>
-    <row r="105" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BL104" s="4"/>
+    </row>
+    <row r="105" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="4"/>
       <c r="B105" s="4"/>
       <c r="C105" s="4"/>
@@ -7918,8 +8074,9 @@
       <c r="BI105" s="4"/>
       <c r="BJ105" s="4"/>
       <c r="BK105" s="4"/>
-    </row>
-    <row r="106" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BL105" s="4"/>
+    </row>
+    <row r="106" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="4"/>
       <c r="B106" s="4"/>
       <c r="C106" s="4"/>
@@ -7983,8 +8140,9 @@
       <c r="BI106" s="4"/>
       <c r="BJ106" s="4"/>
       <c r="BK106" s="4"/>
-    </row>
-    <row r="107" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BL106" s="4"/>
+    </row>
+    <row r="107" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="4"/>
       <c r="B107" s="4"/>
       <c r="C107" s="4"/>
@@ -8048,8 +8206,9 @@
       <c r="BI107" s="4"/>
       <c r="BJ107" s="4"/>
       <c r="BK107" s="4"/>
-    </row>
-    <row r="108" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BL107" s="4"/>
+    </row>
+    <row r="108" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="4"/>
       <c r="B108" s="4"/>
       <c r="C108" s="4"/>
@@ -8113,8 +8272,9 @@
       <c r="BI108" s="4"/>
       <c r="BJ108" s="4"/>
       <c r="BK108" s="4"/>
-    </row>
-    <row r="109" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BL108" s="4"/>
+    </row>
+    <row r="109" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="4"/>
       <c r="B109" s="4"/>
       <c r="C109" s="4"/>
@@ -8178,8 +8338,9 @@
       <c r="BI109" s="4"/>
       <c r="BJ109" s="4"/>
       <c r="BK109" s="4"/>
-    </row>
-    <row r="110" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BL109" s="4"/>
+    </row>
+    <row r="110" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="4"/>
       <c r="B110" s="4"/>
       <c r="C110" s="4"/>
@@ -8243,8 +8404,9 @@
       <c r="BI110" s="4"/>
       <c r="BJ110" s="4"/>
       <c r="BK110" s="4"/>
-    </row>
-    <row r="111" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BL110" s="4"/>
+    </row>
+    <row r="111" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="4"/>
       <c r="B111" s="4"/>
       <c r="C111" s="4"/>
@@ -8308,8 +8470,9 @@
       <c r="BI111" s="4"/>
       <c r="BJ111" s="4"/>
       <c r="BK111" s="4"/>
-    </row>
-    <row r="112" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BL111" s="4"/>
+    </row>
+    <row r="112" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="4"/>
       <c r="B112" s="4"/>
       <c r="C112" s="4"/>
@@ -8373,8 +8536,9 @@
       <c r="BI112" s="4"/>
       <c r="BJ112" s="4"/>
       <c r="BK112" s="4"/>
-    </row>
-    <row r="113" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BL112" s="4"/>
+    </row>
+    <row r="113" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A113" s="4"/>
       <c r="B113" s="4"/>
       <c r="C113" s="4"/>
@@ -8438,8 +8602,9 @@
       <c r="BI113" s="4"/>
       <c r="BJ113" s="4"/>
       <c r="BK113" s="4"/>
-    </row>
-    <row r="114" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BL113" s="4"/>
+    </row>
+    <row r="114" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="4"/>
       <c r="B114" s="4"/>
       <c r="C114" s="4"/>
@@ -8503,8 +8668,9 @@
       <c r="BI114" s="4"/>
       <c r="BJ114" s="4"/>
       <c r="BK114" s="4"/>
-    </row>
-    <row r="115" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BL114" s="4"/>
+    </row>
+    <row r="115" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A115" s="4"/>
       <c r="B115" s="4"/>
       <c r="C115" s="4"/>
@@ -8568,8 +8734,9 @@
       <c r="BI115" s="4"/>
       <c r="BJ115" s="4"/>
       <c r="BK115" s="4"/>
-    </row>
-    <row r="116" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BL115" s="4"/>
+    </row>
+    <row r="116" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A116" s="4"/>
       <c r="B116" s="4"/>
       <c r="C116" s="4"/>
@@ -8633,8 +8800,9 @@
       <c r="BI116" s="4"/>
       <c r="BJ116" s="4"/>
       <c r="BK116" s="4"/>
-    </row>
-    <row r="117" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BL116" s="4"/>
+    </row>
+    <row r="117" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A117" s="4"/>
       <c r="B117" s="4"/>
       <c r="C117" s="4"/>
@@ -8698,8 +8866,9 @@
       <c r="BI117" s="4"/>
       <c r="BJ117" s="4"/>
       <c r="BK117" s="4"/>
-    </row>
-    <row r="118" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BL117" s="4"/>
+    </row>
+    <row r="118" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A118" s="4"/>
       <c r="B118" s="4"/>
       <c r="C118" s="4"/>
@@ -8763,8 +8932,9 @@
       <c r="BI118" s="4"/>
       <c r="BJ118" s="4"/>
       <c r="BK118" s="4"/>
-    </row>
-    <row r="119" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BL118" s="4"/>
+    </row>
+    <row r="119" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A119" s="4"/>
       <c r="B119" s="4"/>
       <c r="C119" s="4"/>
@@ -8828,8 +8998,9 @@
       <c r="BI119" s="4"/>
       <c r="BJ119" s="4"/>
       <c r="BK119" s="4"/>
-    </row>
-    <row r="120" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BL119" s="4"/>
+    </row>
+    <row r="120" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A120" s="4"/>
       <c r="B120" s="4"/>
       <c r="C120" s="4"/>
@@ -8893,8 +9064,9 @@
       <c r="BI120" s="4"/>
       <c r="BJ120" s="4"/>
       <c r="BK120" s="4"/>
-    </row>
-    <row r="121" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BL120" s="4"/>
+    </row>
+    <row r="121" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A121" s="4"/>
       <c r="B121" s="4"/>
       <c r="C121" s="4"/>
@@ -8958,8 +9130,9 @@
       <c r="BI121" s="4"/>
       <c r="BJ121" s="4"/>
       <c r="BK121" s="4"/>
-    </row>
-    <row r="122" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BL121" s="4"/>
+    </row>
+    <row r="122" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A122" s="4"/>
       <c r="B122" s="4"/>
       <c r="C122" s="4"/>
@@ -9023,8 +9196,9 @@
       <c r="BI122" s="4"/>
       <c r="BJ122" s="4"/>
       <c r="BK122" s="4"/>
-    </row>
-    <row r="123" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BL122" s="4"/>
+    </row>
+    <row r="123" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A123" s="4"/>
       <c r="B123" s="4"/>
       <c r="C123" s="4"/>
@@ -9088,8 +9262,9 @@
       <c r="BI123" s="4"/>
       <c r="BJ123" s="4"/>
       <c r="BK123" s="4"/>
-    </row>
-    <row r="124" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BL123" s="4"/>
+    </row>
+    <row r="124" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A124" s="4"/>
       <c r="B124" s="4"/>
       <c r="C124" s="4"/>
@@ -9153,8 +9328,9 @@
       <c r="BI124" s="4"/>
       <c r="BJ124" s="4"/>
       <c r="BK124" s="4"/>
-    </row>
-    <row r="125" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BL124" s="4"/>
+    </row>
+    <row r="125" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A125" s="4"/>
       <c r="B125" s="4"/>
       <c r="C125" s="4"/>
@@ -9218,8 +9394,9 @@
       <c r="BI125" s="4"/>
       <c r="BJ125" s="4"/>
       <c r="BK125" s="4"/>
-    </row>
-    <row r="126" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BL125" s="4"/>
+    </row>
+    <row r="126" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A126" s="4"/>
       <c r="B126" s="4"/>
       <c r="C126" s="4"/>
@@ -9283,8 +9460,9 @@
       <c r="BI126" s="4"/>
       <c r="BJ126" s="4"/>
       <c r="BK126" s="4"/>
-    </row>
-    <row r="127" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BL126" s="4"/>
+    </row>
+    <row r="127" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A127" s="4"/>
       <c r="B127" s="4"/>
       <c r="C127" s="4"/>
@@ -9348,8 +9526,9 @@
       <c r="BI127" s="4"/>
       <c r="BJ127" s="4"/>
       <c r="BK127" s="4"/>
-    </row>
-    <row r="128" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BL127" s="4"/>
+    </row>
+    <row r="128" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A128" s="4"/>
       <c r="B128" s="4"/>
       <c r="C128" s="4"/>
@@ -9413,8 +9592,9 @@
       <c r="BI128" s="4"/>
       <c r="BJ128" s="4"/>
       <c r="BK128" s="4"/>
-    </row>
-    <row r="129" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BL128" s="4"/>
+    </row>
+    <row r="129" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A129" s="4"/>
       <c r="B129" s="4"/>
       <c r="C129" s="4"/>
@@ -9478,14 +9658,15 @@
       <c r="BI129" s="4"/>
       <c r="BJ129" s="4"/>
       <c r="BK129" s="4"/>
+      <c r="BL129" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Expt 2 also done
</commit_message>
<xml_diff>
--- a/COBREX-CLI/finaleval.xlsx
+++ b/COBREX-CLI/finaleval.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="166">
   <si>
     <t xml:space="preserve">Sr.No.</t>
   </si>
@@ -605,6 +606,50 @@
   </si>
   <si>
     <t xml:space="preserve">FUELSAVE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATM_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATM_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATM_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STRAIGHT-FLAG
+FLUSH-FLAG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATM_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CARD-VALUE
+CARD-SUIT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATM_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATM_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CARD-VALUE(I)
+CARD-VALUE(J)
+CARD-SUIT(I)
+CARD-SUIT(J)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATM_7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATM_8</t>
   </si>
 </sst>
 </file>
@@ -700,28 +745,28 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -729,11 +774,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -760,8 +809,8 @@
   </sheetPr>
   <dimension ref="A1:BP129"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10498,4 +10547,117 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <f aca="false">-C5</f>
+        <v>-0</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Final updates on the eval file
</commit_message>
<xml_diff>
--- a/COBREX-CLI/finaleval.xlsx
+++ b/COBREX-CLI/finaleval.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="172">
   <si>
     <t xml:space="preserve">Sr.No.</t>
   </si>
@@ -365,6 +365,11 @@
     <t xml:space="preserve">{'end-if': {'Branch-Logic', 'Sequential-Logic'}, 'if': {'Branch-Logic', 'Sequential-Logic'}, 'set': {'Branch-Logic', 'Sequential-Logic'}, 'rule': {'Sequential-Logic'}, 'paragraphName': {'Sequential-Logic'}}</t>
   </si>
   <si>
+    <t xml:space="preserve">-&gt; 18 are computation rules
+-&gt; 7 rules are realised as one big check input rule
+-&gt; When trigger rule is fetching separate rules instead of encapsulating them as one</t>
+  </si>
+  <si>
     <t xml:space="preserve">AESXGET.cbl</t>
   </si>
   <si>
@@ -379,7 +384,10 @@
     <t xml:space="preserve">{'open', 'close', 'start', 'read', 'continue', 'evaluate', 'goback', 'string', 'paragraphName'}</t>
   </si>
   <si>
-    <t xml:space="preserve">{'end-if': {'Branch-Logic'}, 'if': {'Branch-Logic'}, 'perform': {'Branch-Logic'}, 'move': {'Branch-Logic'}, 'call': {'Branch-Logic'}, 'set': {'Branch-Logic'}}</t>
+    <t xml:space="preserve">BranchLogic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-&gt; We are saying if evaluate then it is a rule why?</t>
   </si>
   <si>
     <t xml:space="preserve">CWKTCOBX.cbl</t>
@@ -535,6 +543,12 @@
     <t xml:space="preserve">{'perform': {'Branch-Logic'}, 'if': {'Branch-Logic', 'Sequential-Logic'}, 'end-if': {'Branch-Logic', 'Sequential-Logic'}, 'move': {'Branch-Logic', 'Sequential-Logic'}, 'rule': {'Branch-Logic', 'Sequential-Logic'}, 'display': {'Branch-Logic', 'Sequential-Logic'}, 'call': {'Branch-Logic', 'Sequential-Logic'}, 'open': {'Sequential-Logic'}, 'paragraphName': {'Sequential-Logic'}, 'start': {'Sequential-Logic'}}</t>
   </si>
   <si>
+    <t xml:space="preserve">Sequential Logic. Branch Logic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-&gt; Doubtful of the CFG but the thing is all the rules are realised but not merged to  appropriate level</t>
+  </si>
+  <si>
     <t xml:space="preserve">eleve.cob</t>
   </si>
   <si>
@@ -562,6 +576,12 @@
   </si>
   <si>
     <t xml:space="preserve">{'accept': {'Loop-Logic', 'Sequential-Logic'}, 'display': {'Loop-Logic', 'Sequential-Logic'}, 'perform': {'Loop-Logic', 'Sequential-Logic'}, 'rule': {'Loop-Logic', 'Sequential-Logic'}, 'paragraphName': {'Sequential-Logic'}, 'set': {'Sequential-Logic'}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sequential Logic. Loop Logic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-&gt; when separate trigger</t>
   </si>
   <si>
     <t xml:space="preserve">FAKPERS.cob</t>
@@ -745,7 +765,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -786,10 +806,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -809,8 +825,8 @@
   </sheetPr>
   <dimension ref="A1:BP129"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U1" activeCellId="0" sqref="U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -968,9 +984,8 @@
         <f aca="false">(I2/G2)*100</f>
         <v>0</v>
       </c>
-      <c r="U2" s="4" t="e">
-        <f aca="false">(2*S2*T2)/(S2+T2)</f>
-        <v>#DIV/0!</v>
+      <c r="U2" s="4" t="n">
+        <v>0</v>
       </c>
       <c r="V2" s="7"/>
       <c r="W2" s="4"/>
@@ -1076,17 +1091,15 @@
       <c r="R3" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="S3" s="4" t="e">
-        <f aca="false">(I3/K3)*100</f>
-        <v>#DIV/0!</v>
+      <c r="S3" s="4" t="n">
+        <v>0</v>
       </c>
       <c r="T3" s="4" t="n">
         <f aca="false">(I3/G3)*100</f>
         <v>0</v>
       </c>
-      <c r="U3" s="4" t="e">
-        <f aca="false">(2*S3*T3)/(S3+T3)</f>
-        <v>#DIV/0!</v>
+      <c r="U3" s="4" t="n">
+        <v>0</v>
       </c>
       <c r="V3" s="4"/>
       <c r="W3" s="4"/>
@@ -1430,9 +1443,8 @@
         <f aca="false">(I6/G6)*100</f>
         <v>0</v>
       </c>
-      <c r="U6" s="4" t="e">
-        <f aca="false">(2*S6*T6)/(S6+T6)</f>
-        <v>#DIV/0!</v>
+      <c r="U6" s="4" t="n">
+        <v>0</v>
       </c>
       <c r="V6" s="4"/>
       <c r="W6" s="4"/>
@@ -1654,13 +1666,11 @@
         <f aca="false">(I8/K8)*100</f>
         <v>0</v>
       </c>
-      <c r="T8" s="4" t="e">
-        <f aca="false">(I8/G8)*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U8" s="4" t="e">
-        <f aca="false">(2*S8*T8)/(S8+T8)</f>
-        <v>#DIV/0!</v>
+      <c r="T8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="U8" s="4" t="n">
+        <v>0</v>
       </c>
       <c r="V8" s="4"/>
       <c r="W8" s="4"/>
@@ -2070,15 +2080,21 @@
         <v>93</v>
       </c>
       <c r="E12" s="5"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
+      <c r="F12" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="G12" s="4" t="n">
+        <v>27</v>
+      </c>
       <c r="H12" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="I12" s="4"/>
+      <c r="I12" s="4" t="n">
+        <v>1</v>
+      </c>
       <c r="J12" s="4" t="n">
         <f aca="false">K12-I12</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K12" s="4" t="n">
         <v>5</v>
@@ -2099,22 +2115,26 @@
       <c r="Q12" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="R12" s="4"/>
+      <c r="R12" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="S12" s="4" t="n">
         <f aca="false">(I12/K12)*100</f>
-        <v>0</v>
-      </c>
-      <c r="T12" s="4" t="e">
+        <v>20</v>
+      </c>
+      <c r="T12" s="4" t="n">
         <f aca="false">(I12/G12)*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U12" s="4" t="e">
+        <v>3.7037037037037</v>
+      </c>
+      <c r="U12" s="4" t="n">
         <f aca="false">(2*S12*T12)/(S12+T12)</f>
-        <v>#DIV/0!</v>
+        <v>6.25</v>
       </c>
       <c r="V12" s="4"/>
       <c r="W12" s="4"/>
-      <c r="X12" s="4"/>
+      <c r="X12" s="8" t="s">
+        <v>97</v>
+      </c>
       <c r="Y12" s="4"/>
       <c r="Z12" s="4"/>
       <c r="AA12" s="4"/>
@@ -2160,39 +2180,45 @@
       <c r="BO12" s="8"/>
       <c r="BP12" s="8"/>
     </row>
-    <row r="13" customFormat="false" ht="72.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="148.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="n">
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C13" s="4" t="n">
         <v>10</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E13" s="5"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
+      <c r="F13" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="H13" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="I13" s="4"/>
+      <c r="I13" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="J13" s="4" t="n">
         <f aca="false">K13-I13</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K13" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L13" s="4"/>
       <c r="M13" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="O13" s="4" t="n">
         <v>14</v>
@@ -2201,24 +2227,24 @@
         <v>55</v>
       </c>
       <c r="Q13" s="4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="R13" s="4"/>
       <c r="S13" s="4" t="n">
         <f aca="false">(I13/K13)*100</f>
         <v>0</v>
       </c>
-      <c r="T13" s="4" t="e">
-        <f aca="false">(I13/G13)*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U13" s="4" t="e">
-        <f aca="false">(2*S13*T13)/(S13+T13)</f>
-        <v>#DIV/0!</v>
+      <c r="T13" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="U13" s="4" t="n">
+        <v>0</v>
       </c>
       <c r="V13" s="4"/>
       <c r="W13" s="4"/>
-      <c r="X13" s="4"/>
+      <c r="X13" s="4" t="s">
+        <v>103</v>
+      </c>
       <c r="Y13" s="4"/>
       <c r="Z13" s="4"/>
       <c r="AA13" s="4"/>
@@ -2264,41 +2290,47 @@
       <c r="BO13" s="8"/>
       <c r="BP13" s="8"/>
     </row>
-    <row r="14" customFormat="false" ht="645.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="193" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="n">
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C14" s="4" t="n">
         <v>52</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
+        <v>106</v>
+      </c>
+      <c r="F14" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="G14" s="4" t="n">
+        <v>4</v>
+      </c>
       <c r="H14" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="I14" s="4"/>
+      <c r="I14" s="4" t="n">
+        <v>1</v>
+      </c>
       <c r="J14" s="4" t="n">
         <f aca="false">K14-I14</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K14" s="4" t="n">
         <v>10</v>
       </c>
       <c r="L14" s="4"/>
       <c r="M14" s="4" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="O14" s="4" t="n">
         <v>15</v>
@@ -2307,20 +2339,22 @@
         <v>212</v>
       </c>
       <c r="Q14" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="R14" s="4"/>
+        <v>109</v>
+      </c>
+      <c r="R14" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="S14" s="4" t="n">
         <f aca="false">(I14/K14)*100</f>
-        <v>0</v>
-      </c>
-      <c r="T14" s="4" t="e">
+        <v>10</v>
+      </c>
+      <c r="T14" s="4" t="n">
         <f aca="false">(I14/G14)*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U14" s="4" t="e">
+        <v>25</v>
+      </c>
+      <c r="U14" s="4" t="n">
         <f aca="false">(2*S14*T14)/(S14+T14)</f>
-        <v>#DIV/0!</v>
+        <v>14.2857142857143</v>
       </c>
       <c r="V14" s="4"/>
       <c r="W14" s="4"/>
@@ -2370,41 +2404,47 @@
       <c r="BO14" s="8"/>
       <c r="BP14" s="8"/>
     </row>
-    <row r="15" customFormat="false" ht="431.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="159.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="n">
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C15" s="4" t="n">
         <v>23</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
+        <v>112</v>
+      </c>
+      <c r="F15" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="G15" s="4" t="n">
+        <v>3</v>
+      </c>
       <c r="H15" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="I15" s="4"/>
+      <c r="I15" s="4" t="n">
+        <v>3</v>
+      </c>
       <c r="J15" s="4" t="n">
         <f aca="false">K15-I15</f>
         <v>3</v>
       </c>
       <c r="K15" s="4" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L15" s="4"/>
       <c r="M15" s="4" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="N15" s="4" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="O15" s="4" t="n">
         <v>15</v>
@@ -2413,20 +2453,22 @@
         <v>69</v>
       </c>
       <c r="Q15" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="R15" s="4"/>
+        <v>115</v>
+      </c>
+      <c r="R15" s="4" t="s">
+        <v>57</v>
+      </c>
       <c r="S15" s="4" t="n">
         <f aca="false">(I15/K15)*100</f>
-        <v>0</v>
-      </c>
-      <c r="T15" s="4" t="e">
+        <v>50</v>
+      </c>
+      <c r="T15" s="4" t="n">
         <f aca="false">(I15/G15)*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U15" s="4" t="e">
+        <v>100</v>
+      </c>
+      <c r="U15" s="4" t="n">
         <f aca="false">(2*S15*T15)/(S15+T15)</f>
-        <v>#DIV/0!</v>
+        <v>66.6666666666667</v>
       </c>
       <c r="V15" s="4"/>
       <c r="W15" s="4"/>
@@ -2476,41 +2518,47 @@
       <c r="BO15" s="8"/>
       <c r="BP15" s="8"/>
     </row>
-    <row r="16" customFormat="false" ht="431.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="178.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="n">
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C16" s="4" t="n">
         <v>51</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
+        <v>112</v>
+      </c>
+      <c r="F16" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="G16" s="4" t="n">
+        <v>3</v>
+      </c>
       <c r="H16" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="I16" s="4"/>
+      <c r="I16" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="J16" s="4" t="n">
         <f aca="false">K16-I16</f>
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="K16" s="4" t="n">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="L16" s="4"/>
       <c r="M16" s="4" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="N16" s="4" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="O16" s="4" t="n">
         <v>16</v>
@@ -2519,20 +2567,21 @@
         <v>147</v>
       </c>
       <c r="Q16" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="R16" s="4"/>
+        <v>119</v>
+      </c>
+      <c r="R16" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="S16" s="4" t="n">
         <f aca="false">(I16/K16)*100</f>
         <v>0</v>
       </c>
-      <c r="T16" s="4" t="e">
+      <c r="T16" s="4" t="n">
         <f aca="false">(I16/G16)*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U16" s="4" t="e">
-        <f aca="false">(2*S16*T16)/(S16+T16)</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
+      </c>
+      <c r="U16" s="4" t="n">
+        <v>0</v>
       </c>
       <c r="V16" s="4"/>
       <c r="W16" s="4"/>
@@ -2587,23 +2636,29 @@
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C17" s="4" t="n">
         <v>20</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
+        <v>122</v>
+      </c>
+      <c r="F17" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="G17" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="H17" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="I17" s="4"/>
+      <c r="I17" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="J17" s="4" t="n">
         <f aca="false">K17-I17</f>
         <v>4</v>
@@ -2613,10 +2668,10 @@
       </c>
       <c r="L17" s="4"/>
       <c r="M17" s="4" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="N17" s="4" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="O17" s="4" t="n">
         <v>13</v>
@@ -2625,20 +2680,20 @@
         <v>62</v>
       </c>
       <c r="Q17" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="R17" s="4"/>
+        <v>125</v>
+      </c>
+      <c r="R17" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="S17" s="4" t="n">
         <f aca="false">(I17/K17)*100</f>
         <v>0</v>
       </c>
-      <c r="T17" s="4" t="e">
-        <f aca="false">(I17/G17)*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U17" s="4" t="e">
-        <f aca="false">(2*S17*T17)/(S17+T17)</f>
-        <v>#DIV/0!</v>
+      <c r="T17" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="U17" s="4" t="n">
+        <v>0</v>
       </c>
       <c r="V17" s="4"/>
       <c r="W17" s="4"/>
@@ -2693,36 +2748,42 @@
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C18" s="4" t="n">
         <v>46</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
+        <v>128</v>
+      </c>
+      <c r="F18" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G18" s="4" t="n">
+        <v>3</v>
+      </c>
       <c r="H18" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="I18" s="4"/>
+      <c r="I18" s="4" t="n">
+        <v>3</v>
+      </c>
       <c r="J18" s="4" t="n">
         <f aca="false">K18-I18</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K18" s="4" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="L18" s="4"/>
       <c r="M18" s="4" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="N18" s="4" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="O18" s="4" t="n">
         <v>13</v>
@@ -2733,18 +2794,20 @@
       <c r="Q18" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="R18" s="4"/>
+      <c r="R18" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="S18" s="4" t="n">
         <f aca="false">(I18/K18)*100</f>
-        <v>0</v>
-      </c>
-      <c r="T18" s="4" t="e">
+        <v>50</v>
+      </c>
+      <c r="T18" s="4" t="n">
         <f aca="false">(I18/G18)*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U18" s="4" t="e">
+        <v>100</v>
+      </c>
+      <c r="U18" s="4" t="n">
         <f aca="false">(2*S18*T18)/(S18+T18)</f>
-        <v>#DIV/0!</v>
+        <v>66.6666666666667</v>
       </c>
       <c r="V18" s="4"/>
       <c r="W18" s="4"/>
@@ -2799,23 +2862,29 @@
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C19" s="4" t="n">
         <v>112</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
+        <v>133</v>
+      </c>
+      <c r="F19" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="G19" s="4" t="n">
+        <v>5</v>
+      </c>
       <c r="H19" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="I19" s="4"/>
+      <c r="I19" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="J19" s="4" t="n">
         <f aca="false">K19-I19</f>
         <v>24</v>
@@ -2825,10 +2894,10 @@
       </c>
       <c r="L19" s="4"/>
       <c r="M19" s="4" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="N19" s="4" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="O19" s="4" t="n">
         <v>13</v>
@@ -2837,24 +2906,27 @@
         <v>327</v>
       </c>
       <c r="Q19" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="R19" s="4"/>
+        <v>136</v>
+      </c>
+      <c r="R19" s="4" t="s">
+        <v>137</v>
+      </c>
       <c r="S19" s="4" t="n">
         <f aca="false">(I19/K19)*100</f>
         <v>0</v>
       </c>
-      <c r="T19" s="4" t="e">
+      <c r="T19" s="4" t="n">
         <f aca="false">(I19/G19)*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U19" s="4" t="e">
-        <f aca="false">(2*S19*T19)/(S19+T19)</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
+      </c>
+      <c r="U19" s="4" t="n">
+        <v>0</v>
       </c>
       <c r="V19" s="4"/>
       <c r="W19" s="4"/>
-      <c r="X19" s="4"/>
+      <c r="X19" s="4" t="s">
+        <v>138</v>
+      </c>
       <c r="Y19" s="4"/>
       <c r="Z19" s="4"/>
       <c r="AA19" s="4"/>
@@ -2905,36 +2977,42 @@
         <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="C20" s="4" t="n">
         <v>48</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
+        <v>141</v>
+      </c>
+      <c r="F20" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" s="4" t="n">
+        <v>8</v>
+      </c>
       <c r="H20" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="I20" s="4"/>
+      <c r="I20" s="4" t="n">
+        <v>7</v>
+      </c>
       <c r="J20" s="4" t="n">
         <f aca="false">K20-I20</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K20" s="4" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="L20" s="4"/>
       <c r="M20" s="4" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="N20" s="4" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="O20" s="4" t="n">
         <v>19</v>
@@ -2943,24 +3021,28 @@
         <v>132</v>
       </c>
       <c r="Q20" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="R20" s="4"/>
+        <v>144</v>
+      </c>
+      <c r="R20" s="4" t="s">
+        <v>145</v>
+      </c>
       <c r="S20" s="4" t="n">
         <f aca="false">(I20/K20)*100</f>
-        <v>0</v>
-      </c>
-      <c r="T20" s="4" t="e">
+        <v>70</v>
+      </c>
+      <c r="T20" s="4" t="n">
         <f aca="false">(I20/G20)*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U20" s="4" t="e">
+        <v>87.5</v>
+      </c>
+      <c r="U20" s="4" t="n">
         <f aca="false">(2*S20*T20)/(S20+T20)</f>
-        <v>#DIV/0!</v>
+        <v>77.7777777777778</v>
       </c>
       <c r="V20" s="4"/>
       <c r="W20" s="4"/>
-      <c r="X20" s="4"/>
+      <c r="X20" s="4" t="s">
+        <v>146</v>
+      </c>
       <c r="Y20" s="4"/>
       <c r="Z20" s="4"/>
       <c r="AA20" s="4"/>
@@ -3011,16 +3093,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="C21" s="4" t="n">
         <v>122</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
@@ -3037,10 +3119,10 @@
       </c>
       <c r="L21" s="4"/>
       <c r="M21" s="4" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="N21" s="4" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="O21" s="4" t="n">
         <v>17</v>
@@ -3049,20 +3131,18 @@
         <v>267</v>
       </c>
       <c r="Q21" s="4" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="R21" s="4"/>
       <c r="S21" s="4" t="n">
         <f aca="false">(I21/K21)*100</f>
         <v>0</v>
       </c>
-      <c r="T21" s="4" t="e">
-        <f aca="false">(I21/G21)*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U21" s="4" t="e">
-        <f aca="false">(2*S21*T21)/(S21+T21)</f>
-        <v>#DIV/0!</v>
+      <c r="T21" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="U21" s="4" t="n">
+        <v>0</v>
       </c>
       <c r="V21" s="4"/>
       <c r="W21" s="4"/>
@@ -3131,9 +3211,18 @@
       <c r="P22" s="4"/>
       <c r="Q22" s="4"/>
       <c r="R22" s="4"/>
-      <c r="S22" s="4"/>
-      <c r="T22" s="4"/>
-      <c r="U22" s="4"/>
+      <c r="S22" s="4" t="n">
+        <f aca="false">AVERAGE(S2:S21)</f>
+        <v>28.8214285714286</v>
+      </c>
+      <c r="T22" s="4" t="n">
+        <f aca="false">AVERAGE(T2:T21)</f>
+        <v>37.5601851851852</v>
+      </c>
+      <c r="U22" s="4" t="n">
+        <f aca="false">AVERAGE(U2:U21)</f>
+        <v>31.2013888888889</v>
+      </c>
       <c r="V22" s="4"/>
       <c r="W22" s="4"/>
       <c r="X22" s="4"/>
@@ -3185,14 +3274,14 @@
     <row r="23" customFormat="false" ht="135.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="4"/>
       <c r="B23" s="4" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="9" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
@@ -3261,7 +3350,7 @@
     <row r="24" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="4"/>
       <c r="B24" s="4" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -3333,7 +3422,7 @@
     <row r="25" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="4"/>
       <c r="B25" s="4" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -3405,7 +3494,7 @@
     <row r="26" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="4"/>
       <c r="B26" s="4" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
@@ -3477,7 +3566,7 @@
     <row r="27" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="4"/>
       <c r="B27" s="4" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
@@ -10556,98 +10645,98 @@
   </sheetPr>
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>155</v>
+      <c r="A1" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>154</v>
+      <c r="A2" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="B3" s="10" t="s">
+      <c r="A3" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>158</v>
+      <c r="C3" s="9" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>160</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>158</v>
+      <c r="A4" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="B5" s="0" t="n">
+      <c r="A5" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B5" s="1" t="n">
         <f aca="false">-C5</f>
         <v>-0</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>158</v>
+      <c r="A6" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="B7" s="0" t="n">
+      <c r="A7" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B7" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="B8" s="10" t="s">
+      <c r="A8" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B8" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="1" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Table 1 and 2 done 19 programs
</commit_message>
<xml_diff>
--- a/COBREX-CLI/finaleval.xlsx
+++ b/COBREX-CLI/finaleval.xlsx
@@ -924,7 +924,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -986,10 +986,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11113,9 +11109,9 @@
   <dimension ref="A1:Z28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
+      <selection pane="bottomLeft" activeCell="S9" activeCellId="0" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11132,7 +11128,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="12.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="12.65"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="13" style="10" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="33.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="33.75"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11278,6 +11274,16 @@
         <f aca="false">(O3/N3)*100</f>
         <v>85.7142857142857</v>
       </c>
+      <c r="Q3" s="0" t="n">
+        <f aca="false">F3</f>
+        <v>4</v>
+      </c>
+      <c r="R3" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="S3" s="0" t="n">
+        <v>75</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="73.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="n">
@@ -11329,6 +11335,16 @@
         <f aca="false">(O4/N4)*100</f>
         <v>0</v>
       </c>
+      <c r="Q4" s="0" t="n">
+        <f aca="false">F4</f>
+        <v>6</v>
+      </c>
+      <c r="R4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="V4" s="1" t="s">
         <v>190</v>
       </c>
@@ -11383,6 +11399,16 @@
         <f aca="false">(O5/N5)*100</f>
         <v>91.3793103448276</v>
       </c>
+      <c r="Q5" s="0" t="n">
+        <f aca="false">F5</f>
+        <v>12</v>
+      </c>
+      <c r="R5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S5" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="77.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="n">
@@ -11434,6 +11460,16 @@
         <f aca="false">(O6/N6)*100</f>
         <v>75.9259259259259</v>
       </c>
+      <c r="Q6" s="0" t="n">
+        <f aca="false">F6</f>
+        <v>5</v>
+      </c>
+      <c r="R6" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="S6" s="0" t="n">
+        <v>60</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="72.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="n">
@@ -11485,6 +11521,16 @@
         <f aca="false">(O7/N7)*100</f>
         <v>0</v>
       </c>
+      <c r="Q7" s="0" t="n">
+        <f aca="false">F7</f>
+        <v>1</v>
+      </c>
+      <c r="R7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="V7" s="1" t="s">
         <v>191</v>
       </c>
@@ -11539,6 +11585,16 @@
         <f aca="false">(O8/N8)*100</f>
         <v>100</v>
       </c>
+      <c r="Q8" s="0" t="n">
+        <f aca="false">F8</f>
+        <v>1</v>
+      </c>
+      <c r="R8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S8" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="n">
@@ -11589,6 +11645,16 @@
       <c r="P9" s="1" t="n">
         <v>100</v>
       </c>
+      <c r="Q9" s="0" t="n">
+        <f aca="false">F9</f>
+        <v>0</v>
+      </c>
+      <c r="R9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S9" s="0" t="n">
+        <v>100</v>
+      </c>
       <c r="V9" s="14" t="s">
         <v>192</v>
       </c>
@@ -11643,6 +11709,16 @@
         <f aca="false">(O10/N10)*100</f>
         <v>14.2857142857143</v>
       </c>
+      <c r="Q10" s="0" t="n">
+        <f aca="false">F10</f>
+        <v>1</v>
+      </c>
+      <c r="R10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S10" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="V10" s="15" t="s">
         <v>193</v>
       </c>
@@ -11697,6 +11773,16 @@
         <f aca="false">(O11/N11)*100</f>
         <v>100</v>
       </c>
+      <c r="Q11" s="0" t="n">
+        <f aca="false">F11</f>
+        <v>3</v>
+      </c>
+      <c r="R11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S11" s="0" t="n">
+        <v>100</v>
+      </c>
       <c r="V11" s="14" t="s">
         <v>194</v>
       </c>
@@ -11749,6 +11835,16 @@
       </c>
       <c r="P12" s="1" t="n">
         <f aca="false">(O12/N12)*100</f>
+        <v>100</v>
+      </c>
+      <c r="Q12" s="0" t="n">
+        <f aca="false">F12</f>
+        <v>5</v>
+      </c>
+      <c r="R12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S12" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -11805,6 +11901,18 @@
         <f aca="false">(O13/N13)*100</f>
         <v>89.0282131661442</v>
       </c>
+      <c r="Q13" s="0" t="n">
+        <f aca="false">F13</f>
+        <v>9</v>
+      </c>
+      <c r="R13" s="0" t="n">
+        <f aca="false">700/9</f>
+        <v>77.7777777777778</v>
+      </c>
+      <c r="S13" s="0" t="n">
+        <f aca="false">200/9</f>
+        <v>22.2222222222222</v>
+      </c>
       <c r="V13" s="15" t="s">
         <v>195</v>
       </c>
@@ -11860,6 +11968,16 @@
       <c r="P14" s="1" t="n">
         <v>100</v>
       </c>
+      <c r="Q14" s="0" t="n">
+        <f aca="false">F14</f>
+        <v>0</v>
+      </c>
+      <c r="R14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S14" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="93.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="n">
@@ -11911,6 +12029,16 @@
         <f aca="false">(O15/N15)*100</f>
         <v>29.0322580645161</v>
       </c>
+      <c r="Q15" s="0" t="n">
+        <f aca="false">F15</f>
+        <v>4</v>
+      </c>
+      <c r="R15" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="S15" s="0" t="n">
+        <v>25</v>
+      </c>
       <c r="V15" s="1" t="s">
         <v>197</v>
       </c>
@@ -11965,6 +12093,16 @@
         <f aca="false">(O16/N16)*100</f>
         <v>100</v>
       </c>
+      <c r="Q16" s="0" t="n">
+        <f aca="false">F16</f>
+        <v>3</v>
+      </c>
+      <c r="R16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S16" s="0" t="n">
+        <v>100</v>
+      </c>
       <c r="V16" s="1" t="s">
         <v>198</v>
       </c>
@@ -12009,17 +12147,29 @@
         <f aca="false">(2*J17*K17)/(J17+K17)</f>
         <v>13.3333333333333</v>
       </c>
-      <c r="N17" s="0" t="n">
-        <f aca="false">4+59+14+14+2+28</f>
-        <v>121</v>
-      </c>
-      <c r="O17" s="0" t="n">
+      <c r="N17" s="1" t="n">
+        <f aca="false">5+59+14+14+2+28</f>
+        <v>122</v>
+      </c>
+      <c r="O17" s="1" t="n">
         <f aca="false">36+14+14+28</f>
         <v>92</v>
       </c>
       <c r="P17" s="1" t="n">
         <f aca="false">(O17/N17)*100</f>
-        <v>76.0330578512397</v>
+        <v>75.4098360655738</v>
+      </c>
+      <c r="Q17" s="0" t="n">
+        <f aca="false">F17</f>
+        <v>3</v>
+      </c>
+      <c r="R17" s="0" t="n">
+        <f aca="false">100/3</f>
+        <v>33.3333333333333</v>
+      </c>
+      <c r="S17" s="0" t="n">
+        <f aca="false">200/3</f>
+        <v>66.6666666666667</v>
       </c>
       <c r="V17" s="1" t="s">
         <v>199</v>
@@ -12065,13 +12215,23 @@
         <f aca="false">(2*J18*K18)/(J18+K18)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N18" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="O18" s="0" t="n">
+      <c r="N18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O18" s="1" t="n">
         <v>0</v>
       </c>
       <c r="P18" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="Q18" s="0" t="n">
+        <f aca="false">F18</f>
+        <v>0</v>
+      </c>
+      <c r="R18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S18" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -12115,11 +12275,11 @@
         <f aca="false">(2*J19*K19)/(J19+K19)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N19" s="0" t="n">
+      <c r="N19" s="1" t="n">
         <f aca="false">7+39+7+58+7+64</f>
         <v>182</v>
       </c>
-      <c r="O19" s="0" t="n">
+      <c r="O19" s="1" t="n">
         <f aca="false">39+58+64</f>
         <v>161</v>
       </c>
@@ -12128,15 +12288,16 @@
         <v>88.4615384615385</v>
       </c>
       <c r="Q19" s="0" t="n">
+        <f aca="false">F19</f>
         <v>3</v>
       </c>
-      <c r="R19" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="S19" s="0" t="n">
+      <c r="R19" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S19" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="V19" s="16" t="s">
+      <c r="V19" s="9" t="s">
         <v>200</v>
       </c>
     </row>
@@ -12183,11 +12344,11 @@
         <f aca="false">(2*J20*K20)/(J20+K20)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N20" s="0" t="n">
+      <c r="N20" s="1" t="n">
         <f aca="false">60+32+123+21+12</f>
         <v>248</v>
       </c>
-      <c r="O20" s="0" t="n">
+      <c r="O20" s="1" t="n">
         <f aca="false">30+18+64+0+0</f>
         <v>112</v>
       </c>
@@ -12195,14 +12356,14 @@
         <f aca="false">(O20/N20)*100</f>
         <v>45.1612903225806</v>
       </c>
-      <c r="Q20" s="0" t="n">
+      <c r="Q20" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="R20" s="0" t="n">
+      <c r="R20" s="1" t="n">
         <f aca="false">(2/Q20)*100</f>
         <v>40</v>
       </c>
-      <c r="S20" s="0" t="n">
+      <c r="S20" s="1" t="n">
         <v>60</v>
       </c>
     </row>
@@ -12246,11 +12407,11 @@
         <f aca="false">(2*J21*K21)/(J21+K21)</f>
         <v>36.3636363636364</v>
       </c>
-      <c r="N21" s="0" t="n">
+      <c r="N21" s="1" t="n">
         <f aca="false">19+2+28</f>
         <v>49</v>
       </c>
-      <c r="O21" s="0" t="n">
+      <c r="O21" s="1" t="n">
         <f aca="false">19+2+28</f>
         <v>49</v>
       </c>
@@ -12258,16 +12419,16 @@
         <f aca="false">(O21/N21)*100</f>
         <v>100</v>
       </c>
-      <c r="Q21" s="0" t="n">
+      <c r="Q21" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="R21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="S21" s="0" t="n">
+      <c r="R21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S21" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="V21" s="0" t="s">
+      <c r="V21" s="1" t="s">
         <v>201</v>
       </c>
     </row>
@@ -12306,9 +12467,9 @@
         <f aca="false">(O22/N22)*100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="V22" s="0" t="n">
+      <c r="V22" s="1" t="n">
         <f aca="false">AVERAGE(P3:P21)</f>
-        <v>73.4221891650933</v>
+        <v>73.3893880184793</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="133.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Evaluation done for 24 programs
</commit_message>
<xml_diff>
--- a/COBREX-CLI/finaleval.xlsx
+++ b/COBREX-CLI/finaleval.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="213">
   <si>
     <t xml:space="preserve">Sr.No.</t>
   </si>
@@ -788,20 +788,28 @@
 GST</t>
   </si>
   <si>
-    <t xml:space="preserve">TOTAL-INCOME
-TOTAL-EXPENSE
-TAXABLE-INCOME
-TAX-AMOUNT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ACCOUNT-BALANCE
-ACCOUNT-TYPE</t>
-  </si>
-  <si>
     <t xml:space="preserve">BMI.cbl</t>
   </si>
   <si>
+    <t xml:space="preserve">BMI
+HEART-RATE
+BLOOD-PRESSURE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEIGHTT
+WEIGHT
+AGE
+GENDER</t>
+  </si>
+  <si>
     <t xml:space="preserve">PRIME.cbl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FLAG
+I</t>
   </si>
 </sst>
 </file>
@@ -924,68 +932,72 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11106,12 +11118,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z28"/>
+  <dimension ref="A1:Z1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="2" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="S9" activeCellId="0" sqref="S9"/>
+      <selection pane="bottomLeft" activeCell="R26" activeCellId="0" sqref="R26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11131,7 +11143,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="33.75"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
         <v>172</v>
       </c>
@@ -11155,7 +11167,7 @@
       <c r="R1" s="11"/>
       <c r="S1" s="11"/>
       <c r="T1" s="12"/>
-      <c r="U1" s="11" t="s">
+      <c r="U1" s="13" t="s">
         <v>174</v>
       </c>
       <c r="V1" s="12"/>
@@ -11274,18 +11286,18 @@
         <f aca="false">(O3/N3)*100</f>
         <v>85.7142857142857</v>
       </c>
-      <c r="Q3" s="0" t="n">
+      <c r="Q3" s="1" t="n">
         <f aca="false">F3</f>
         <v>4</v>
       </c>
-      <c r="R3" s="0" t="n">
+      <c r="R3" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="S3" s="0" t="n">
+      <c r="S3" s="1" t="n">
         <v>75</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="73.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="72.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="n">
         <v>2</v>
       </c>
@@ -11335,21 +11347,21 @@
         <f aca="false">(O4/N4)*100</f>
         <v>0</v>
       </c>
-      <c r="Q4" s="0" t="n">
+      <c r="Q4" s="1" t="n">
         <f aca="false">F4</f>
         <v>6</v>
       </c>
-      <c r="R4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="S4" s="0" t="n">
+      <c r="R4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" s="1" t="n">
         <v>0</v>
       </c>
       <c r="V4" s="1" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="90.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="n">
         <v>3</v>
       </c>
@@ -11399,18 +11411,18 @@
         <f aca="false">(O5/N5)*100</f>
         <v>91.3793103448276</v>
       </c>
-      <c r="Q5" s="0" t="n">
+      <c r="Q5" s="1" t="n">
         <f aca="false">F5</f>
         <v>12</v>
       </c>
-      <c r="R5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="S5" s="0" t="n">
+      <c r="R5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S5" s="1" t="n">
         <v>100</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="77.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="77.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="n">
         <v>4</v>
       </c>
@@ -11460,14 +11472,14 @@
         <f aca="false">(O6/N6)*100</f>
         <v>75.9259259259259</v>
       </c>
-      <c r="Q6" s="0" t="n">
+      <c r="Q6" s="1" t="n">
         <f aca="false">F6</f>
         <v>5</v>
       </c>
-      <c r="R6" s="0" t="n">
+      <c r="R6" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="S6" s="0" t="n">
+      <c r="S6" s="1" t="n">
         <v>60</v>
       </c>
     </row>
@@ -11521,14 +11533,14 @@
         <f aca="false">(O7/N7)*100</f>
         <v>0</v>
       </c>
-      <c r="Q7" s="0" t="n">
+      <c r="Q7" s="1" t="n">
         <f aca="false">F7</f>
         <v>1</v>
       </c>
-      <c r="R7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="S7" s="0" t="n">
+      <c r="R7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" s="1" t="n">
         <v>0</v>
       </c>
       <c r="V7" s="1" t="s">
@@ -11585,14 +11597,14 @@
         <f aca="false">(O8/N8)*100</f>
         <v>100</v>
       </c>
-      <c r="Q8" s="0" t="n">
+      <c r="Q8" s="1" t="n">
         <f aca="false">F8</f>
         <v>1</v>
       </c>
-      <c r="R8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="S8" s="0" t="n">
+      <c r="R8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S8" s="1" t="n">
         <v>100</v>
       </c>
     </row>
@@ -11609,10 +11621,10 @@
       <c r="D9" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="E9" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" s="13" t="n">
+      <c r="E9" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="14" t="n">
         <v>0</v>
       </c>
       <c r="G9" s="1" t="n">
@@ -11645,17 +11657,17 @@
       <c r="P9" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="Q9" s="0" t="n">
+      <c r="Q9" s="1" t="n">
         <f aca="false">F9</f>
         <v>0</v>
       </c>
-      <c r="R9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="S9" s="0" t="n">
+      <c r="R9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S9" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="V9" s="14" t="s">
+      <c r="V9" s="15" t="s">
         <v>192</v>
       </c>
     </row>
@@ -11709,17 +11721,17 @@
         <f aca="false">(O10/N10)*100</f>
         <v>14.2857142857143</v>
       </c>
-      <c r="Q10" s="0" t="n">
+      <c r="Q10" s="1" t="n">
         <f aca="false">F10</f>
         <v>1</v>
       </c>
-      <c r="R10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="S10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V10" s="15" t="s">
+      <c r="R10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="V10" s="16" t="s">
         <v>193</v>
       </c>
     </row>
@@ -11773,21 +11785,21 @@
         <f aca="false">(O11/N11)*100</f>
         <v>100</v>
       </c>
-      <c r="Q11" s="0" t="n">
+      <c r="Q11" s="1" t="n">
         <f aca="false">F11</f>
         <v>3</v>
       </c>
-      <c r="R11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="S11" s="0" t="n">
+      <c r="R11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S11" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="V11" s="14" t="s">
+      <c r="V11" s="15" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="95.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="95.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="n">
         <v>10</v>
       </c>
@@ -11837,18 +11849,18 @@
         <f aca="false">(O12/N12)*100</f>
         <v>100</v>
       </c>
-      <c r="Q12" s="0" t="n">
+      <c r="Q12" s="1" t="n">
         <f aca="false">F12</f>
         <v>5</v>
       </c>
-      <c r="R12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="S12" s="0" t="n">
+      <c r="R12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S12" s="1" t="n">
         <v>100</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="88.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="87.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="n">
         <v>11</v>
       </c>
@@ -11901,22 +11913,22 @@
         <f aca="false">(O13/N13)*100</f>
         <v>89.0282131661442</v>
       </c>
-      <c r="Q13" s="0" t="n">
+      <c r="Q13" s="1" t="n">
         <f aca="false">F13</f>
         <v>9</v>
       </c>
-      <c r="R13" s="0" t="n">
+      <c r="R13" s="1" t="n">
         <f aca="false">700/9</f>
         <v>77.7777777777778</v>
       </c>
-      <c r="S13" s="0" t="n">
+      <c r="S13" s="1" t="n">
         <f aca="false">200/9</f>
         <v>22.2222222222222</v>
       </c>
-      <c r="V13" s="15" t="s">
+      <c r="V13" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="Y13" s="13" t="s">
+      <c r="Y13" s="14" t="s">
         <v>196</v>
       </c>
     </row>
@@ -11968,18 +11980,18 @@
       <c r="P14" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="Q14" s="0" t="n">
+      <c r="Q14" s="1" t="n">
         <f aca="false">F14</f>
         <v>0</v>
       </c>
-      <c r="R14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="S14" s="0" t="n">
+      <c r="R14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S14" s="1" t="n">
         <v>100</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="93.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="93" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="n">
         <v>13</v>
       </c>
@@ -12029,21 +12041,21 @@
         <f aca="false">(O15/N15)*100</f>
         <v>29.0322580645161</v>
       </c>
-      <c r="Q15" s="0" t="n">
+      <c r="Q15" s="1" t="n">
         <f aca="false">F15</f>
         <v>4</v>
       </c>
-      <c r="R15" s="0" t="n">
+      <c r="R15" s="1" t="n">
         <v>75</v>
       </c>
-      <c r="S15" s="0" t="n">
+      <c r="S15" s="1" t="n">
         <v>25</v>
       </c>
       <c r="V15" s="1" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="89.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="89.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="n">
         <v>14</v>
       </c>
@@ -12093,21 +12105,21 @@
         <f aca="false">(O16/N16)*100</f>
         <v>100</v>
       </c>
-      <c r="Q16" s="0" t="n">
+      <c r="Q16" s="1" t="n">
         <f aca="false">F16</f>
         <v>3</v>
       </c>
-      <c r="R16" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="S16" s="0" t="n">
+      <c r="R16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S16" s="1" t="n">
         <v>100</v>
       </c>
       <c r="V16" s="1" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="81.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="81" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="n">
         <v>15</v>
       </c>
@@ -12159,15 +12171,15 @@
         <f aca="false">(O17/N17)*100</f>
         <v>75.4098360655738</v>
       </c>
-      <c r="Q17" s="0" t="n">
+      <c r="Q17" s="1" t="n">
         <f aca="false">F17</f>
         <v>3</v>
       </c>
-      <c r="R17" s="0" t="n">
+      <c r="R17" s="1" t="n">
         <f aca="false">100/3</f>
         <v>33.3333333333333</v>
       </c>
-      <c r="S17" s="0" t="n">
+      <c r="S17" s="1" t="n">
         <f aca="false">200/3</f>
         <v>66.6666666666667</v>
       </c>
@@ -12224,14 +12236,14 @@
       <c r="P18" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="Q18" s="0" t="n">
+      <c r="Q18" s="1" t="n">
         <f aca="false">F18</f>
         <v>0</v>
       </c>
-      <c r="R18" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="S18" s="0" t="n">
+      <c r="R18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S18" s="1" t="n">
         <v>100</v>
       </c>
     </row>
@@ -12287,7 +12299,7 @@
         <f aca="false">(O19/N19)*100</f>
         <v>88.4615384615385</v>
       </c>
-      <c r="Q19" s="0" t="n">
+      <c r="Q19" s="1" t="n">
         <f aca="false">F19</f>
         <v>3</v>
       </c>
@@ -12301,7 +12313,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="80.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="79.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="n">
         <v>18</v>
       </c>
@@ -12367,7 +12379,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="139.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="138.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="n">
         <v>19</v>
       </c>
@@ -12432,122 +12444,347 @@
         <v>201</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="126.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="92.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="n">
         <v>20</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>140</v>
+        <v>152</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E22" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="G22" s="1" t="n">
-        <v>94</v>
+        <v>6</v>
+      </c>
+      <c r="H22" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="I22" s="1" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="J22" s="1" t="n">
         <f aca="false">(H22/I22)*100</f>
-        <v>0</v>
-      </c>
-      <c r="K22" s="1" t="e">
+        <v>50</v>
+      </c>
+      <c r="K22" s="1" t="n">
         <f aca="false">(H22/F22)*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L22" s="1" t="e">
+        <v>100</v>
+      </c>
+      <c r="L22" s="1" t="n">
         <f aca="false">(2*J22*K22)/(J22+K22)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P22" s="1" t="e">
-        <f aca="false">(O22/N22)*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V22" s="1" t="n">
-        <f aca="false">AVERAGE(P3:P21)</f>
-        <v>73.3893880184793</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="133.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>66.6666666666667</v>
+      </c>
+      <c r="N22" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="O22" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="P22" s="1" t="n">
+        <f aca="false">O22*100/N22</f>
+        <v>100</v>
+      </c>
+      <c r="Q22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S22" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="73.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="n">
         <v>21</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>155</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="E23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F23" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="G23" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="H23" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I23" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="J23" s="1" t="n">
+        <f aca="false">(H23/I23)*100</f>
+        <v>0</v>
+      </c>
+      <c r="K23" s="1" t="n">
+        <f aca="false">(H23/F23)*100</f>
+        <v>0</v>
+      </c>
+      <c r="L23" s="1" t="e">
+        <f aca="false">(2*J23*K23)/(J23+K23)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N23" s="0" t="n">
+        <f aca="false">21+21+44+13</f>
+        <v>99</v>
+      </c>
+      <c r="O23" s="0" t="n">
+        <f aca="false">0+0+44+13</f>
+        <v>57</v>
+      </c>
+      <c r="P23" s="1" t="n">
+        <f aca="false">(O23/N23)*100</f>
+        <v>57.5757575757576</v>
+      </c>
+      <c r="Q23" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="R23" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="S23" s="0" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="91.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="n">
         <v>22</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>156</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="E24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="G24" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="H24" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="I24" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="J24" s="1" t="n">
+        <f aca="false">(H24/I24)*100</f>
+        <v>83.3333333333333</v>
+      </c>
+      <c r="K24" s="1" t="n">
+        <f aca="false">(H24/F24)*100</f>
+        <v>100</v>
+      </c>
+      <c r="L24" s="1" t="n">
+        <f aca="false">(2*J24*K24)/(J24+K24)</f>
+        <v>90.9090909090909</v>
+      </c>
+      <c r="N24" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="O24" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="P24" s="1" t="n">
+        <f aca="false">(O24/N24)*100</f>
+        <v>100</v>
+      </c>
+      <c r="Q24" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="R24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S24" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="108.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="n">
         <v>23</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>205</v>
+        <v>207</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>208</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="144.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>209</v>
+      </c>
+      <c r="E25" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G25" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="H25" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I25" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J25" s="1" t="n">
+        <f aca="false">(H25/I25)*100</f>
+        <v>50</v>
+      </c>
+      <c r="K25" s="1" t="n">
+        <f aca="false">(H25/F25)*100</f>
+        <v>50</v>
+      </c>
+      <c r="L25" s="1" t="n">
+        <f aca="false">(2*J25*K25)/(J25+K25)</f>
+        <v>50</v>
+      </c>
+      <c r="N25" s="0" t="n">
+        <f aca="false">11+13</f>
+        <v>24</v>
+      </c>
+      <c r="O25" s="0" t="n">
+        <f aca="false">7+12</f>
+        <v>19</v>
+      </c>
+      <c r="P25" s="1" t="n">
+        <f aca="false">O25*100/N25</f>
+        <v>79.1666666666667</v>
+      </c>
+      <c r="Q25" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="R25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S25" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="n">
         <v>24</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>157</v>
+        <v>210</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>212</v>
+      </c>
+      <c r="E26" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G26" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H26" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I26" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J26" s="1" t="n">
+        <f aca="false">(H26/I26)*100</f>
+        <v>100</v>
+      </c>
+      <c r="K26" s="1" t="n">
+        <f aca="false">(H26/F26)*100</f>
+        <v>100</v>
+      </c>
+      <c r="L26" s="1" t="n">
+        <f aca="false">(2*J26*K26)/(J26+K26)</f>
+        <v>100</v>
+      </c>
+      <c r="N26" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="O26" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="P26" s="1" t="n">
+        <f aca="false">(O26/N26)*100</f>
+        <v>100</v>
+      </c>
+      <c r="Q26" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S26" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="126.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="n">
         <v>25</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-    </row>
-    <row r="28" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="4" t="n">
-        <v>26</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-    </row>
+        <v>147</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="G27" s="1" t="n">
+        <v>94</v>
+      </c>
+      <c r="I27" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="J27" s="1" t="n">
+        <f aca="false">(H27/I27)*100</f>
+        <v>0</v>
+      </c>
+      <c r="K27" s="1" t="e">
+        <f aca="false">(H27/F27)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L27" s="1" t="e">
+        <f aca="false">(2*J27*K27)/(J27+K27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P27" s="1" t="e">
+        <f aca="false">(O27/N27)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:L1"/>

</xml_diff>